<commit_message>
1,2 tabs draft done.  3rd tab date and ticker working
</commit_message>
<xml_diff>
--- a/Stock_Parser/demo.xlsx
+++ b/Stock_Parser/demo.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8970" windowWidth="21570" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8970" windowWidth="21570" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="8_29_2018 Stock List" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Daily Stock List" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cumulative_Stock_List" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Price Changes" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Stock Additions</t>
   </si>
@@ -47,36 +48,36 @@
     <t>CRON</t>
   </si>
   <si>
+    <t>AMD</t>
+  </si>
+  <si>
     <t>AMZN</t>
   </si>
   <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>TQQQ</t>
+  </si>
+  <si>
     <t>TLRY</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>AMD</t>
-  </si>
-  <si>
-    <t>FB</t>
-  </si>
-  <si>
-    <t>NVDA</t>
-  </si>
-  <si>
-    <t>TQQQ</t>
-  </si>
-  <si>
     <t>MSFT</t>
   </si>
   <si>
-    <t>CRM</t>
-  </si>
-  <si>
     <t>SPY</t>
   </si>
   <si>
@@ -138,6 +139,12 @@
   </si>
   <si>
     <t>DKS</t>
+  </si>
+  <si>
+    <t>8/30/2018</t>
+  </si>
+  <si>
+    <t>Goog</t>
   </si>
 </sst>
 </file>
@@ -145,7 +152,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="20">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -189,15 +196,78 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FF00"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FF00"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF00B050"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FF00"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FF00"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <color rgb="00FF0000"/>
+    </font>
+    <font>
       <color rgb="0000FF00"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -222,6 +292,20 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -500,7 +584,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -541,22 +625,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>12.74</v>
-      </c>
-      <c s="8" r="C4" t="n">
-        <v>1.66</v>
-      </c>
-      <c s="8" r="D4" t="n">
-        <v>13.03</v>
+        <v>11.31</v>
+      </c>
+      <c s="21" r="C4" t="n">
+        <v>-1.43</v>
+      </c>
+      <c s="21" r="D4" t="n">
+        <v>-12.64</v>
       </c>
       <c r="E4" t="n">
-        <v>2240</v>
+        <v>804</v>
       </c>
       <c r="F4" t="n">
-        <v>1400</v>
-      </c>
-      <c s="8" r="G4" t="n">
-        <v>0.62</v>
+        <v>395</v>
+      </c>
+      <c s="22" r="G4" t="n">
+        <v>0.67</v>
       </c>
       <c r="H4" t="n">
         <v>3.95</v>
@@ -567,25 +651,25 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>1998.1</v>
-      </c>
-      <c s="8" r="C5" t="n">
-        <v>65.28</v>
-      </c>
-      <c s="8" r="D5" t="n">
-        <v>3.27</v>
+        <v>25.25</v>
+      </c>
+      <c s="22" r="C5" t="n">
+        <v>0.05</v>
+      </c>
+      <c s="22" r="D5" t="n">
+        <v>0.2</v>
       </c>
       <c r="E5" t="n">
-        <v>2791</v>
+        <v>537</v>
       </c>
       <c r="F5" t="n">
-        <v>2724</v>
-      </c>
-      <c s="8" r="G5" t="n">
-        <v>0.51</v>
+        <v>375</v>
+      </c>
+      <c s="22" r="G5" t="n">
+        <v>0.59</v>
       </c>
       <c r="H5" t="n">
-        <v>1.61</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -593,48 +677,48 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>62.13</v>
-      </c>
-      <c s="8" r="C6" t="n">
-        <v>10.63</v>
-      </c>
-      <c s="8" r="D6" t="n">
-        <v>17.11</v>
+        <v>2001.13</v>
+      </c>
+      <c s="22" r="C6" t="n">
+        <v>3.03</v>
+      </c>
+      <c s="22" r="D6" t="n">
+        <v>0.15</v>
       </c>
       <c r="E6" t="n">
-        <v>2390</v>
+        <v>865</v>
       </c>
       <c r="F6" t="n">
-        <v>1583</v>
-      </c>
-      <c s="8" r="G6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
+        <v>711</v>
+      </c>
+      <c s="22" r="G6" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.61</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>222.98</v>
-      </c>
-      <c s="8" r="C7" t="n">
-        <v>3.28</v>
-      </c>
-      <c s="8" r="D7" t="n">
-        <v>1.47</v>
+        <v>222.97</v>
+      </c>
+      <c s="21" r="C7" t="n">
+        <v>-0.01</v>
+      </c>
+      <c s="22" r="D7" t="n">
+        <v>-0</v>
       </c>
       <c r="E7" t="n">
-        <v>1715</v>
+        <v>656</v>
       </c>
       <c r="F7" t="n">
-        <v>1153</v>
-      </c>
-      <c s="8" r="G7" t="n">
-        <v>0.6</v>
+        <v>394</v>
+      </c>
+      <c s="22" r="G7" t="n">
+        <v>0.62</v>
       </c>
       <c r="H7" t="n">
         <v>1.14</v>
@@ -642,33 +726,33 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>25.2</v>
-      </c>
-      <c s="8" r="C8" t="n">
-        <v>0.15</v>
-      </c>
-      <c s="8" r="D8" t="n">
-        <v>0.6</v>
+        <v>150.19</v>
+      </c>
+      <c s="21" r="C8" t="n">
+        <v>-4.61</v>
+      </c>
+      <c s="21" r="D8" t="n">
+        <v>-3.07</v>
       </c>
       <c r="E8" t="n">
-        <v>2477</v>
+        <v>916</v>
       </c>
       <c r="F8" t="n">
-        <v>2465</v>
-      </c>
-      <c s="8" r="G8" t="n">
-        <v>0.5</v>
+        <v>660</v>
+      </c>
+      <c s="22" r="G8" t="n">
+        <v>0.58</v>
       </c>
       <c r="H8" t="n">
-        <v>3.6</v>
+        <v>1.13</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="n">
         <v>222.98</v>
@@ -720,7 +804,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="n">
         <v>175.9</v>
@@ -746,7 +830,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="n">
         <v>278.49</v>
@@ -772,7 +856,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="n">
         <v>72.5</v>
@@ -798,7 +882,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B14" t="n">
         <v>62.13</v>
@@ -819,12 +903,12 @@
         <v>0.6</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" t="n">
         <v>112.02</v>
@@ -850,7 +934,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B16" t="n">
         <v>154.8</v>
@@ -1006,7 +1090,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B22" t="n">
         <v>25.2</v>
@@ -1053,7 +1137,7 @@
         <v>0.49</v>
       </c>
       <c r="H23" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1162,7 +1246,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B28" t="n">
         <v>1998.1</v>
@@ -1328,9 +1412,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView topLeftCell="A13" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -1541,693 +1625,1843 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>1998.1</v>
-      </c>
-      <c s="8" r="C8" t="n">
-        <v>65.28</v>
-      </c>
-      <c s="8" r="D8" t="n">
-        <v>3.27</v>
+        <v>11.71</v>
+      </c>
+      <c s="9" r="C8" t="n">
+        <v>-1.03</v>
+      </c>
+      <c s="9" r="D8" t="n">
+        <v>-8.800000000000001</v>
       </c>
       <c r="E8" t="n">
-        <v>2791</v>
+        <v>349</v>
       </c>
       <c r="F8" t="n">
-        <v>2724</v>
+        <v>231</v>
       </c>
       <c s="8" r="G8" t="n">
-        <v>0.51</v>
+        <v>0.6</v>
       </c>
       <c r="H8" t="n">
-        <v>1.61</v>
+        <v>3.95</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>1998.1</v>
-      </c>
-      <c s="8" r="C9" t="n">
-        <v>65.28</v>
-      </c>
-      <c s="8" r="D9" t="n">
-        <v>3.27</v>
+        <v>11.6</v>
+      </c>
+      <c s="10" r="C9" t="n">
+        <v>-1.14</v>
+      </c>
+      <c s="10" r="D9" t="n">
+        <v>-9.83</v>
       </c>
       <c r="E9" t="n">
-        <v>2791</v>
+        <v>655</v>
       </c>
       <c r="F9" t="n">
-        <v>2724</v>
-      </c>
-      <c s="8" r="G9" t="n">
-        <v>0.51</v>
+        <v>327</v>
+      </c>
+      <c s="11" r="G9" t="n">
+        <v>0.67</v>
       </c>
       <c r="H9" t="n">
-        <v>1.61</v>
+        <v>3.95</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>62.13</v>
-      </c>
-      <c s="8" r="C10" t="n">
-        <v>10.63</v>
-      </c>
-      <c s="8" r="D10" t="n">
-        <v>17.11</v>
+        <v>11.6</v>
+      </c>
+      <c s="10" r="C10" t="n">
+        <v>-1.14</v>
+      </c>
+      <c s="10" r="D10" t="n">
+        <v>-9.83</v>
       </c>
       <c r="E10" t="n">
-        <v>2390</v>
+        <v>655</v>
       </c>
       <c r="F10" t="n">
-        <v>1583</v>
-      </c>
-      <c s="8" r="G10" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>12</v>
+        <v>327</v>
+      </c>
+      <c s="11" r="G10" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3.95</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>62.13</v>
-      </c>
-      <c s="8" r="C11" t="n">
-        <v>10.63</v>
-      </c>
-      <c s="8" r="D11" t="n">
-        <v>17.11</v>
+        <v>11.48</v>
+      </c>
+      <c s="10" r="C11" t="n">
+        <v>-1.26</v>
+      </c>
+      <c s="10" r="D11" t="n">
+        <v>-10.98</v>
       </c>
       <c r="E11" t="n">
-        <v>2390</v>
+        <v>655</v>
       </c>
       <c r="F11" t="n">
-        <v>1583</v>
-      </c>
-      <c s="8" r="G11" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H11" t="s">
-        <v>12</v>
+        <v>327</v>
+      </c>
+      <c s="11" r="G11" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3.95</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12" t="n">
-        <v>222.98</v>
-      </c>
-      <c s="8" r="C12" t="n">
-        <v>3.28</v>
-      </c>
-      <c s="8" r="D12" t="n">
-        <v>1.47</v>
+        <v>11.52</v>
+      </c>
+      <c s="10" r="C12" t="n">
+        <v>-1.22</v>
+      </c>
+      <c s="10" r="D12" t="n">
+        <v>-10.59</v>
       </c>
       <c r="E12" t="n">
-        <v>1715</v>
+        <v>655</v>
       </c>
       <c r="F12" t="n">
-        <v>1153</v>
-      </c>
-      <c s="8" r="G12" t="n">
-        <v>0.6</v>
+        <v>327</v>
+      </c>
+      <c s="11" r="G12" t="n">
+        <v>0.67</v>
       </c>
       <c r="H12" t="n">
-        <v>1.14</v>
+        <v>3.95</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>222.98</v>
-      </c>
-      <c s="8" r="C13" t="n">
-        <v>3.28</v>
-      </c>
-      <c s="8" r="D13" t="n">
-        <v>1.47</v>
+        <v>11.42</v>
+      </c>
+      <c s="17" r="C13" t="n">
+        <v>-1.32</v>
+      </c>
+      <c s="17" r="D13" t="n">
+        <v>-11.56</v>
       </c>
       <c r="E13" t="n">
-        <v>1715</v>
+        <v>804</v>
       </c>
       <c r="F13" t="n">
-        <v>1153</v>
-      </c>
-      <c s="8" r="G13" t="n">
-        <v>0.6</v>
+        <v>395</v>
+      </c>
+      <c s="18" r="G13" t="n">
+        <v>0.67</v>
       </c>
       <c r="H13" t="n">
-        <v>1.14</v>
+        <v>3.95</v>
       </c>
       <c r="I13" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B14" t="n">
-        <v>25.2</v>
-      </c>
-      <c s="8" r="C14" t="n">
-        <v>0.15</v>
-      </c>
-      <c s="8" r="D14" t="n">
-        <v>0.6</v>
+        <v>11.39</v>
+      </c>
+      <c s="19" r="C14" t="n">
+        <v>-1.35</v>
+      </c>
+      <c s="19" r="D14" t="n">
+        <v>-11.85</v>
       </c>
       <c r="E14" t="n">
-        <v>2477</v>
+        <v>804</v>
       </c>
       <c r="F14" t="n">
-        <v>2465</v>
-      </c>
-      <c s="8" r="G14" t="n">
-        <v>0.5</v>
+        <v>395</v>
+      </c>
+      <c s="20" r="G14" t="n">
+        <v>0.67</v>
       </c>
       <c r="H14" t="n">
-        <v>3.6</v>
+        <v>3.95</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B15" t="n">
+        <v>11.31</v>
+      </c>
+      <c s="21" r="C15" t="n">
+        <v>-1.43</v>
+      </c>
+      <c s="21" r="D15" t="n">
+        <v>-12.64</v>
+      </c>
+      <c r="E15" t="n">
+        <v>804</v>
+      </c>
+      <c r="F15" t="n">
+        <v>395</v>
+      </c>
+      <c s="22" r="G15" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="I15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1998.1</v>
+      </c>
+      <c s="8" r="C16" t="n">
+        <v>65.28</v>
+      </c>
+      <c s="8" r="D16" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2791</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2724</v>
+      </c>
+      <c s="8" r="G16" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1998.1</v>
+      </c>
+      <c s="8" r="C17" t="n">
+        <v>65.28</v>
+      </c>
+      <c s="8" r="D17" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2791</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2724</v>
+      </c>
+      <c s="8" r="G17" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2005.03</v>
+      </c>
+      <c s="8" r="C18" t="n">
+        <v>6.93</v>
+      </c>
+      <c s="8" r="D18" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E18" t="n">
+        <v>322</v>
+      </c>
+      <c r="F18" t="n">
+        <v>320</v>
+      </c>
+      <c s="8" r="G18" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1999.03</v>
+      </c>
+      <c s="11" r="C19" t="n">
+        <v>0.93</v>
+      </c>
+      <c s="11" r="D19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E19" t="n">
+        <v>740</v>
+      </c>
+      <c r="F19" t="n">
+        <v>607</v>
+      </c>
+      <c s="11" r="G19" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H19" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1997.49</v>
+      </c>
+      <c s="10" r="C20" t="n">
+        <v>-0.61</v>
+      </c>
+      <c s="10" r="D20" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="E20" t="n">
+        <v>740</v>
+      </c>
+      <c r="F20" t="n">
+        <v>607</v>
+      </c>
+      <c s="11" r="G20" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1997.93</v>
+      </c>
+      <c s="10" r="C21" t="n">
+        <v>-0.17</v>
+      </c>
+      <c s="10" r="D21" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="E21" t="n">
+        <v>740</v>
+      </c>
+      <c r="F21" t="n">
+        <v>607</v>
+      </c>
+      <c s="11" r="G21" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1999.18</v>
+      </c>
+      <c s="11" r="C22" t="n">
+        <v>1.08</v>
+      </c>
+      <c s="11" r="D22" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E22" t="n">
+        <v>740</v>
+      </c>
+      <c r="F22" t="n">
+        <v>607</v>
+      </c>
+      <c s="11" r="G22" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2002.77</v>
+      </c>
+      <c s="18" r="C23" t="n">
+        <v>4.67</v>
+      </c>
+      <c s="18" r="D23" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E23" t="n">
+        <v>865</v>
+      </c>
+      <c r="F23" t="n">
+        <v>711</v>
+      </c>
+      <c s="18" r="G23" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2002.22</v>
+      </c>
+      <c s="20" r="C24" t="n">
+        <v>4.12</v>
+      </c>
+      <c s="20" r="D24" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="E24" t="n">
+        <v>865</v>
+      </c>
+      <c r="F24" t="n">
+        <v>711</v>
+      </c>
+      <c s="20" r="G24" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2001.13</v>
+      </c>
+      <c s="22" r="C25" t="n">
+        <v>3.03</v>
+      </c>
+      <c s="22" r="D25" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E25" t="n">
+        <v>865</v>
+      </c>
+      <c r="F25" t="n">
+        <v>711</v>
+      </c>
+      <c s="22" r="G25" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="n">
+        <v>62.13</v>
+      </c>
+      <c s="8" r="C26" t="n">
+        <v>10.63</v>
+      </c>
+      <c s="8" r="D26" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2390</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1583</v>
+      </c>
+      <c s="8" r="G26" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H26" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="n">
+        <v>62.13</v>
+      </c>
+      <c s="8" r="C27" t="n">
+        <v>10.63</v>
+      </c>
+      <c s="8" r="D27" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2390</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1583</v>
+      </c>
+      <c s="8" r="G27" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="n">
+        <v>222.98</v>
+      </c>
+      <c s="8" r="C28" t="n">
+        <v>3.28</v>
+      </c>
+      <c s="8" r="D28" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1715</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1153</v>
+      </c>
+      <c s="8" r="G28" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="n">
+        <v>222.98</v>
+      </c>
+      <c s="8" r="C29" t="n">
+        <v>3.28</v>
+      </c>
+      <c s="8" r="D29" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1715</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1153</v>
+      </c>
+      <c s="8" r="G29" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="n">
+        <v>224.43</v>
+      </c>
+      <c s="8" r="C30" t="n">
+        <v>1.45</v>
+      </c>
+      <c s="8" r="D30" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="E30" t="n">
+        <v>272</v>
+      </c>
+      <c r="F30" t="n">
+        <v>186</v>
+      </c>
+      <c s="8" r="G30" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="n">
+        <v>222.76</v>
+      </c>
+      <c s="10" r="C31" t="n">
+        <v>-0.22</v>
+      </c>
+      <c s="10" r="D31" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>568</v>
+      </c>
+      <c r="F31" t="n">
+        <v>345</v>
+      </c>
+      <c s="11" r="G31" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="n">
+        <v>222.8</v>
+      </c>
+      <c s="10" r="C32" t="n">
+        <v>-0.18</v>
+      </c>
+      <c s="10" r="D32" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="E32" t="n">
+        <v>568</v>
+      </c>
+      <c r="F32" t="n">
+        <v>345</v>
+      </c>
+      <c s="11" r="G32" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" t="n">
+        <v>222.76</v>
+      </c>
+      <c s="10" r="C33" t="n">
+        <v>-0.22</v>
+      </c>
+      <c s="10" r="D33" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>568</v>
+      </c>
+      <c r="F33" t="n">
+        <v>345</v>
+      </c>
+      <c s="11" r="G33" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="n">
+        <v>222.43</v>
+      </c>
+      <c s="10" r="C34" t="n">
+        <v>-0.55</v>
+      </c>
+      <c s="10" r="D34" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="E34" t="n">
+        <v>568</v>
+      </c>
+      <c r="F34" t="n">
+        <v>345</v>
+      </c>
+      <c s="11" r="G34" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="n">
+        <v>223.03</v>
+      </c>
+      <c s="18" r="C35" t="n">
+        <v>0.05</v>
+      </c>
+      <c s="18" r="D35" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E35" t="n">
+        <v>656</v>
+      </c>
+      <c r="F35" t="n">
+        <v>394</v>
+      </c>
+      <c s="18" r="G35" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="n">
+        <v>222.91</v>
+      </c>
+      <c s="19" r="C36" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c s="19" r="D36" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="E36" t="n">
+        <v>656</v>
+      </c>
+      <c r="F36" t="n">
+        <v>394</v>
+      </c>
+      <c s="20" r="G36" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="n">
+        <v>222.97</v>
+      </c>
+      <c s="21" r="C37" t="n">
+        <v>-0.01</v>
+      </c>
+      <c s="22" r="D37" t="n">
+        <v>-0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>656</v>
+      </c>
+      <c r="F37" t="n">
+        <v>394</v>
+      </c>
+      <c s="22" r="G37" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="n">
         <v>25.2</v>
       </c>
-      <c s="8" r="C15" t="n">
+      <c s="8" r="C38" t="n">
         <v>0.15</v>
       </c>
-      <c s="8" r="D15" t="n">
+      <c s="8" r="D38" t="n">
         <v>0.6</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E38" t="n">
         <v>2477</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F38" t="n">
         <v>2465</v>
       </c>
-      <c s="8" r="G15" t="n">
+      <c s="8" r="G38" t="n">
         <v>0.5</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H38" t="n">
         <v>3.6</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c s="5" r="C16" t="n"/>
-      <c s="5" r="D16" t="n"/>
-      <c s="5" r="G16" t="n"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c s="6" r="C17" t="n"/>
-      <c s="6" r="D17" t="n"/>
-      <c s="5" r="G17" t="n"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c s="6" r="C18" t="n"/>
-      <c s="6" r="D18" t="n"/>
-      <c s="5" r="G18" t="n"/>
-    </row>
-    <row r="19" spans="1:9">
-      <c s="6" r="C19" t="n"/>
-      <c s="6" r="D19" t="n"/>
-      <c s="6" r="G19" t="n"/>
-    </row>
-    <row r="20" spans="1:9">
-      <c s="7" r="C20" t="n"/>
-      <c s="7" r="D20" t="n"/>
-      <c s="7" r="G20" t="n"/>
-    </row>
-    <row r="21" spans="1:9">
-      <c s="6" r="C21" t="n"/>
-      <c s="6" r="D21" t="n"/>
-      <c s="5" r="G21" t="n"/>
-    </row>
-    <row r="22" spans="1:9">
-      <c s="6" r="C22" t="n"/>
-      <c s="6" r="D22" t="n"/>
-      <c s="6" r="G22" t="n"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c s="6" r="C23" t="n"/>
-      <c s="6" r="D23" t="n"/>
-      <c s="6" r="G23" t="n"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c s="5" r="C24" t="n"/>
-      <c s="5" r="D24" t="n"/>
-      <c s="6" r="G24" t="n"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c s="5" r="C25" t="n"/>
-      <c s="5" r="D25" t="n"/>
-      <c s="6" r="G25" t="n"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c s="5" r="C26" t="n"/>
-      <c s="5" r="D26" t="n"/>
-      <c s="5" r="G26" t="n"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c s="6" r="C27" t="n"/>
-      <c s="6" r="D27" t="n"/>
-      <c s="6" r="G27" t="n"/>
-    </row>
-    <row r="28" spans="1:9">
-      <c s="6" r="C28" t="n"/>
-      <c s="6" r="D28" t="n"/>
-      <c s="6" r="G28" t="n"/>
-    </row>
-    <row r="29" spans="1:9">
-      <c s="7" r="C29" t="n"/>
-      <c s="7" r="D29" t="n"/>
-      <c s="7" r="G29" t="n"/>
-    </row>
-    <row r="30" spans="1:9">
-      <c s="5" r="C30" t="n"/>
-      <c s="5" r="D30" t="n"/>
-      <c s="5" r="G30" t="n"/>
-    </row>
-    <row r="31" spans="1:9">
-      <c s="6" r="C31" t="n"/>
-      <c s="6" r="D31" t="n"/>
-      <c s="5" r="G31" t="n"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c s="6" r="C32" t="n"/>
-      <c s="6" r="D32" t="n"/>
-      <c s="6" r="G32" t="n"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c s="6" r="C33" t="n"/>
-      <c s="6" r="D33" t="n"/>
-      <c s="6" r="G33" t="n"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c s="5" r="C34" t="n"/>
-      <c s="5" r="D34" t="n"/>
-      <c s="6" r="G34" t="n"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c s="6" r="C35" t="n"/>
-      <c s="6" r="D35" t="n"/>
-      <c s="6" r="G35" t="n"/>
-    </row>
-    <row r="36" spans="1:9">
-      <c s="7" r="C36" t="n"/>
-      <c s="7" r="D36" t="n"/>
-      <c s="7" r="G36" t="n"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c s="5" r="C37" t="n"/>
-      <c s="5" r="D37" t="n"/>
-      <c s="6" r="G37" t="n"/>
-    </row>
-    <row r="38" spans="1:9">
-      <c s="6" r="C38" t="n"/>
-      <c s="6" r="D38" t="n"/>
-      <c s="5" r="G38" t="n"/>
-    </row>
     <row r="39" spans="1:9">
-      <c s="6" r="C39" t="n"/>
-      <c s="6" r="D39" t="n"/>
-      <c s="6" r="G39" t="n"/>
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" t="n">
+        <v>25.2</v>
+      </c>
+      <c s="8" r="C39" t="n">
+        <v>0.15</v>
+      </c>
+      <c s="8" r="D39" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2477</v>
+      </c>
+      <c r="F39" t="n">
+        <v>2465</v>
+      </c>
+      <c s="8" r="G39" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I39" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="40" spans="1:9">
-      <c s="6" r="C40" t="n"/>
-      <c s="6" r="D40" t="n"/>
-      <c s="5" r="G40" t="n"/>
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="n">
+        <v>24.98</v>
+      </c>
+      <c s="10" r="C40" t="n">
+        <v>-0.22</v>
+      </c>
+      <c s="10" r="D40" t="n">
+        <v>-0.88</v>
+      </c>
+      <c r="E40" t="n">
+        <v>449</v>
+      </c>
+      <c r="F40" t="n">
+        <v>306</v>
+      </c>
+      <c s="11" r="G40" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H40" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I40" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="41" spans="1:9">
-      <c s="5" r="C41" t="n"/>
-      <c s="5" r="D41" t="n"/>
-      <c s="6" r="G41" t="n"/>
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="n">
+        <v>24.99</v>
+      </c>
+      <c s="10" r="C41" t="n">
+        <v>-0.21</v>
+      </c>
+      <c s="10" r="D41" t="n">
+        <v>-0.84</v>
+      </c>
+      <c r="E41" t="n">
+        <v>449</v>
+      </c>
+      <c r="F41" t="n">
+        <v>306</v>
+      </c>
+      <c s="11" r="G41" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H41" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I41" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="42" spans="1:9">
-      <c s="1" r="C42" t="n"/>
-      <c s="1" r="D42" t="n"/>
-      <c s="2" r="G42" t="n"/>
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="n">
+        <v>25.04</v>
+      </c>
+      <c s="10" r="C42" t="n">
+        <v>-0.16</v>
+      </c>
+      <c s="10" r="D42" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="E42" t="n">
+        <v>449</v>
+      </c>
+      <c r="F42" t="n">
+        <v>306</v>
+      </c>
+      <c s="11" r="G42" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H42" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I42" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="43" spans="1:9">
-      <c s="2" r="C43" t="n"/>
-      <c s="2" r="D43" t="n"/>
-      <c s="2" r="G43" t="n"/>
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="n">
+        <v>25.1</v>
+      </c>
+      <c s="10" r="C43" t="n">
+        <v>-0.1</v>
+      </c>
+      <c s="10" r="D43" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="E43" t="n">
+        <v>449</v>
+      </c>
+      <c r="F43" t="n">
+        <v>306</v>
+      </c>
+      <c s="11" r="G43" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H43" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I43" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="44" spans="1:9">
-      <c s="1" r="C44" t="n"/>
-      <c s="1" r="D44" t="n"/>
-      <c s="2" r="G44" t="n"/>
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="n">
+        <v>25.25</v>
+      </c>
+      <c s="18" r="C44" t="n">
+        <v>0.05</v>
+      </c>
+      <c s="18" r="D44" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E44" t="n">
+        <v>537</v>
+      </c>
+      <c r="F44" t="n">
+        <v>375</v>
+      </c>
+      <c s="18" r="G44" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H44" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I44" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="45" spans="1:9">
-      <c s="2" r="C45" t="n"/>
-      <c s="2" r="D45" t="n"/>
-      <c s="2" r="G45" t="n"/>
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="n">
+        <v>25.33</v>
+      </c>
+      <c s="20" r="C45" t="n">
+        <v>0.13</v>
+      </c>
+      <c s="20" r="D45" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E45" t="n">
+        <v>537</v>
+      </c>
+      <c r="F45" t="n">
+        <v>375</v>
+      </c>
+      <c s="20" r="G45" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H45" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I45" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="46" spans="1:9">
-      <c s="2" r="C46" t="n"/>
-      <c s="2" r="D46" t="n"/>
-      <c s="2" r="G46" t="n"/>
+      <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="n">
+        <v>25.25</v>
+      </c>
+      <c s="22" r="C46" t="n">
+        <v>0.05</v>
+      </c>
+      <c s="22" r="D46" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E46" t="n">
+        <v>537</v>
+      </c>
+      <c r="F46" t="n">
+        <v>375</v>
+      </c>
+      <c s="22" r="G46" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H46" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I46" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="47" spans="1:9">
-      <c s="2" r="C47" t="n"/>
-      <c s="2" r="D47" t="n"/>
-      <c s="2" r="G47" t="n"/>
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" t="n">
+        <v>44.69</v>
+      </c>
+      <c s="9" r="C47" t="n">
+        <v>-1.71</v>
+      </c>
+      <c s="9" r="D47" t="n">
+        <v>-3.83</v>
+      </c>
+      <c r="E47" t="n">
+        <v>255</v>
+      </c>
+      <c r="F47" t="n">
+        <v>147</v>
+      </c>
+      <c s="8" r="G47" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="H47" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="I47" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="48" spans="1:9">
-      <c s="1" r="C48" t="n"/>
-      <c s="1" r="D48" t="n"/>
-      <c s="2" r="G48" t="n"/>
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" t="n">
+        <v>152.61</v>
+      </c>
+      <c s="9" r="C48" t="n">
+        <v>-2.19</v>
+      </c>
+      <c s="9" r="D48" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="E48" t="n">
+        <v>599</v>
+      </c>
+      <c r="F48" t="n">
+        <v>414</v>
+      </c>
+      <c s="8" r="G48" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H48" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I48" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="49" spans="1:9">
-      <c s="3" r="C49" t="n"/>
-      <c s="3" r="D49" t="n"/>
-      <c s="4" r="G49" t="n"/>
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" t="n">
+        <v>150.99</v>
+      </c>
+      <c s="10" r="C49" t="n">
+        <v>-3.81</v>
+      </c>
+      <c s="10" r="D49" t="n">
+        <v>-2.52</v>
+      </c>
+      <c r="E49" t="n">
+        <v>823</v>
+      </c>
+      <c r="F49" t="n">
+        <v>612</v>
+      </c>
+      <c s="11" r="G49" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H49" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I49" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="50" spans="1:9">
-      <c s="4" r="C50" t="n"/>
-      <c s="4" r="D50" t="n"/>
-      <c s="4" r="G50" t="n"/>
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" t="n">
+        <v>150.54</v>
+      </c>
+      <c s="10" r="C50" t="n">
+        <v>-4.25</v>
+      </c>
+      <c s="10" r="D50" t="n">
+        <v>-2.82</v>
+      </c>
+      <c r="E50" t="n">
+        <v>823</v>
+      </c>
+      <c r="F50" t="n">
+        <v>612</v>
+      </c>
+      <c s="11" r="G50" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H50" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I50" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="51" spans="1:9">
-      <c s="3" r="C51" t="n"/>
-      <c s="3" r="D51" t="n"/>
-      <c s="3" r="G51" t="n"/>
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" t="n">
+        <v>150.46</v>
+      </c>
+      <c s="10" r="C51" t="n">
+        <v>-4.34</v>
+      </c>
+      <c s="10" r="D51" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="E51" t="n">
+        <v>823</v>
+      </c>
+      <c r="F51" t="n">
+        <v>612</v>
+      </c>
+      <c s="11" r="G51" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I51" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="52" spans="1:9">
-      <c s="3" r="C52" t="n"/>
-      <c s="3" r="D52" t="n"/>
-      <c s="3" r="G52" t="n"/>
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" t="n">
+        <v>150.12</v>
+      </c>
+      <c s="10" r="C52" t="n">
+        <v>-4.68</v>
+      </c>
+      <c s="10" r="D52" t="n">
+        <v>-3.12</v>
+      </c>
+      <c r="E52" t="n">
+        <v>823</v>
+      </c>
+      <c r="F52" t="n">
+        <v>612</v>
+      </c>
+      <c s="11" r="G52" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I52" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="53" spans="1:9">
-      <c s="4" r="C53" t="n"/>
-      <c s="4" r="D53" t="n"/>
-      <c s="4" r="G53" t="n"/>
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="n">
+        <v>150.31</v>
+      </c>
+      <c s="17" r="C53" t="n">
+        <v>-4.49</v>
+      </c>
+      <c s="17" r="D53" t="n">
+        <v>-2.99</v>
+      </c>
+      <c r="E53" t="n">
+        <v>916</v>
+      </c>
+      <c r="F53" t="n">
+        <v>660</v>
+      </c>
+      <c s="18" r="G53" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I53" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="54" spans="1:9">
-      <c s="4" r="C54" t="n"/>
-      <c s="4" r="D54" t="n"/>
-      <c s="4" r="G54" t="n"/>
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="n">
+        <v>150.17</v>
+      </c>
+      <c s="19" r="C54" t="n">
+        <v>-4.63</v>
+      </c>
+      <c s="19" r="D54" t="n">
+        <v>-3.08</v>
+      </c>
+      <c r="E54" t="n">
+        <v>916</v>
+      </c>
+      <c r="F54" t="n">
+        <v>660</v>
+      </c>
+      <c s="20" r="G54" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I54" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="55" spans="1:9">
-      <c s="4" r="C55" t="n"/>
-      <c s="4" r="D55" t="n"/>
-      <c s="4" r="G55" t="n"/>
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" t="n">
+        <v>150.19</v>
+      </c>
+      <c s="21" r="C55" t="n">
+        <v>-4.61</v>
+      </c>
+      <c s="21" r="D55" t="n">
+        <v>-3.07</v>
+      </c>
+      <c r="E55" t="n">
+        <v>916</v>
+      </c>
+      <c r="F55" t="n">
+        <v>660</v>
+      </c>
+      <c s="22" r="G55" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I55" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="56" spans="1:9">
-      <c s="3" r="C56" t="n"/>
-      <c s="3" r="D56" t="n"/>
-      <c s="3" r="G56" t="n"/>
+      <c s="6" r="C56" t="n"/>
+      <c s="6" r="D56" t="n"/>
+      <c s="5" r="G56" t="n"/>
     </row>
     <row r="57" spans="1:9">
-      <c s="4" r="C57" t="n"/>
-      <c s="4" r="D57" t="n"/>
-      <c s="3" r="G57" t="n"/>
+      <c s="6" r="C57" t="n"/>
+      <c s="6" r="D57" t="n"/>
+      <c s="6" r="G57" t="n"/>
     </row>
     <row r="58" spans="1:9">
-      <c s="4" r="C58" t="n"/>
-      <c s="4" r="D58" t="n"/>
-      <c s="3" r="G58" t="n"/>
+      <c s="7" r="C58" t="n"/>
+      <c s="7" r="D58" t="n"/>
+      <c s="7" r="G58" t="n"/>
     </row>
     <row r="59" spans="1:9">
-      <c s="4" r="C59" t="n"/>
-      <c s="4" r="D59" t="n"/>
-      <c s="4" r="G59" t="n"/>
+      <c s="6" r="C59" t="n"/>
+      <c s="6" r="D59" t="n"/>
+      <c s="5" r="G59" t="n"/>
     </row>
     <row r="60" spans="1:9">
-      <c s="4" r="C60" t="n"/>
-      <c s="4" r="D60" t="n"/>
-      <c s="3" r="G60" t="n"/>
+      <c s="6" r="C60" t="n"/>
+      <c s="6" r="D60" t="n"/>
+      <c s="6" r="G60" t="n"/>
     </row>
     <row r="61" spans="1:9">
-      <c s="4" r="C61" t="n"/>
-      <c s="4" r="D61" t="n"/>
-      <c s="4" r="G61" t="n"/>
+      <c s="6" r="C61" t="n"/>
+      <c s="6" r="D61" t="n"/>
+      <c s="6" r="G61" t="n"/>
     </row>
     <row r="62" spans="1:9">
-      <c s="4" r="C62" t="n"/>
-      <c s="4" r="D62" t="n"/>
-      <c s="4" r="G62" t="n"/>
+      <c s="5" r="C62" t="n"/>
+      <c s="5" r="D62" t="n"/>
+      <c s="6" r="G62" t="n"/>
     </row>
     <row r="63" spans="1:9">
-      <c s="3" r="C63" t="n"/>
-      <c s="3" r="D63" t="n"/>
-      <c s="4" r="G63" t="n"/>
+      <c s="5" r="C63" t="n"/>
+      <c s="5" r="D63" t="n"/>
+      <c s="6" r="G63" t="n"/>
     </row>
     <row r="64" spans="1:9">
-      <c s="3" r="C64" t="n"/>
-      <c s="3" r="D64" t="n"/>
-      <c s="4" r="G64" t="n"/>
+      <c s="5" r="C64" t="n"/>
+      <c s="5" r="D64" t="n"/>
+      <c s="5" r="G64" t="n"/>
     </row>
     <row r="65" spans="1:9">
-      <c s="3" r="C65" t="n"/>
-      <c s="3" r="D65" t="n"/>
-      <c s="3" r="G65" t="n"/>
+      <c s="6" r="C65" t="n"/>
+      <c s="6" r="D65" t="n"/>
+      <c s="6" r="G65" t="n"/>
     </row>
     <row r="66" spans="1:9">
-      <c s="4" r="C66" t="n"/>
-      <c s="4" r="D66" t="n"/>
-      <c s="4" r="G66" t="n"/>
+      <c s="6" r="C66" t="n"/>
+      <c s="6" r="D66" t="n"/>
+      <c s="6" r="G66" t="n"/>
     </row>
     <row r="67" spans="1:9">
-      <c s="4" r="C67" t="n"/>
-      <c s="4" r="D67" t="n"/>
-      <c s="4" r="G67" t="n"/>
+      <c s="7" r="C67" t="n"/>
+      <c s="7" r="D67" t="n"/>
+      <c s="7" r="G67" t="n"/>
     </row>
     <row r="68" spans="1:9">
-      <c s="3" r="C68" t="n"/>
-      <c s="3" r="D68" t="n"/>
-      <c s="3" r="G68" t="n"/>
+      <c s="5" r="C68" t="n"/>
+      <c s="5" r="D68" t="n"/>
+      <c s="5" r="G68" t="n"/>
     </row>
     <row r="69" spans="1:9">
-      <c s="4" r="C69" t="n"/>
-      <c s="4" r="D69" t="n"/>
-      <c s="3" r="G69" t="n"/>
+      <c s="6" r="C69" t="n"/>
+      <c s="6" r="D69" t="n"/>
+      <c s="5" r="G69" t="n"/>
     </row>
     <row r="70" spans="1:9">
-      <c s="4" r="C70" t="n"/>
-      <c s="4" r="D70" t="n"/>
-      <c s="4" r="G70" t="n"/>
+      <c s="6" r="C70" t="n"/>
+      <c s="6" r="D70" t="n"/>
+      <c s="6" r="G70" t="n"/>
     </row>
     <row r="71" spans="1:9">
-      <c s="4" r="C71" t="n"/>
-      <c s="4" r="D71" t="n"/>
-      <c s="4" r="G71" t="n"/>
+      <c s="6" r="C71" t="n"/>
+      <c s="6" r="D71" t="n"/>
+      <c s="6" r="G71" t="n"/>
     </row>
     <row r="72" spans="1:9">
-      <c s="3" r="C72" t="n"/>
-      <c s="3" r="D72" t="n"/>
-      <c s="4" r="G72" t="n"/>
+      <c s="5" r="C72" t="n"/>
+      <c s="5" r="D72" t="n"/>
+      <c s="6" r="G72" t="n"/>
     </row>
     <row r="73" spans="1:9">
-      <c s="4" r="C73" t="n"/>
-      <c s="4" r="D73" t="n"/>
-      <c s="4" r="G73" t="n"/>
+      <c s="6" r="C73" t="n"/>
+      <c s="6" r="D73" t="n"/>
+      <c s="6" r="G73" t="n"/>
     </row>
     <row r="74" spans="1:9">
-      <c s="3" r="C74" t="n"/>
-      <c s="3" r="D74" t="n"/>
-      <c s="4" r="G74" t="n"/>
+      <c s="7" r="C74" t="n"/>
+      <c s="7" r="D74" t="n"/>
+      <c s="7" r="G74" t="n"/>
     </row>
     <row r="75" spans="1:9">
-      <c s="4" r="C75" t="n"/>
-      <c s="4" r="D75" t="n"/>
-      <c s="3" r="G75" t="n"/>
+      <c s="5" r="C75" t="n"/>
+      <c s="5" r="D75" t="n"/>
+      <c s="6" r="G75" t="n"/>
     </row>
     <row r="76" spans="1:9">
-      <c s="4" r="C76" t="n"/>
-      <c s="4" r="D76" t="n"/>
-      <c s="4" r="G76" t="n"/>
+      <c s="6" r="C76" t="n"/>
+      <c s="6" r="D76" t="n"/>
+      <c s="5" r="G76" t="n"/>
     </row>
     <row r="77" spans="1:9">
-      <c s="4" r="C77" t="n"/>
-      <c s="4" r="D77" t="n"/>
-      <c s="3" r="G77" t="n"/>
+      <c s="6" r="C77" t="n"/>
+      <c s="6" r="D77" t="n"/>
+      <c s="6" r="G77" t="n"/>
     </row>
     <row r="78" spans="1:9">
-      <c s="3" r="C78" t="n"/>
-      <c s="3" r="D78" t="n"/>
-      <c s="4" r="G78" t="n"/>
+      <c s="6" r="C78" t="n"/>
+      <c s="6" r="D78" t="n"/>
+      <c s="5" r="G78" t="n"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" t="s">
+      <c s="5" r="C79" t="n"/>
+      <c s="5" r="D79" t="n"/>
+      <c s="6" r="G79" t="n"/>
+    </row>
+    <row r="80" spans="1:9">
+      <c s="1" r="C80" t="n"/>
+      <c s="1" r="D80" t="n"/>
+      <c s="2" r="G80" t="n"/>
+    </row>
+    <row r="81" spans="1:9">
+      <c s="2" r="C81" t="n"/>
+      <c s="2" r="D81" t="n"/>
+      <c s="2" r="G81" t="n"/>
+    </row>
+    <row r="82" spans="1:9">
+      <c s="1" r="C82" t="n"/>
+      <c s="1" r="D82" t="n"/>
+      <c s="2" r="G82" t="n"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c s="2" r="C83" t="n"/>
+      <c s="2" r="D83" t="n"/>
+      <c s="2" r="G83" t="n"/>
+    </row>
+    <row r="84" spans="1:9">
+      <c s="2" r="C84" t="n"/>
+      <c s="2" r="D84" t="n"/>
+      <c s="2" r="G84" t="n"/>
+    </row>
+    <row r="85" spans="1:9">
+      <c s="2" r="C85" t="n"/>
+      <c s="2" r="D85" t="n"/>
+      <c s="2" r="G85" t="n"/>
+    </row>
+    <row r="86" spans="1:9">
+      <c s="1" r="C86" t="n"/>
+      <c s="1" r="D86" t="n"/>
+      <c s="2" r="G86" t="n"/>
+    </row>
+    <row r="87" spans="1:9">
+      <c s="3" r="C87" t="n"/>
+      <c s="3" r="D87" t="n"/>
+      <c s="4" r="G87" t="n"/>
+    </row>
+    <row r="88" spans="1:9">
+      <c s="4" r="C88" t="n"/>
+      <c s="4" r="D88" t="n"/>
+      <c s="4" r="G88" t="n"/>
+    </row>
+    <row r="89" spans="1:9">
+      <c s="3" r="C89" t="n"/>
+      <c s="3" r="D89" t="n"/>
+      <c s="3" r="G89" t="n"/>
+    </row>
+    <row r="90" spans="1:9">
+      <c s="3" r="C90" t="n"/>
+      <c s="3" r="D90" t="n"/>
+      <c s="3" r="G90" t="n"/>
+    </row>
+    <row r="91" spans="1:9">
+      <c s="4" r="C91" t="n"/>
+      <c s="4" r="D91" t="n"/>
+      <c s="4" r="G91" t="n"/>
+    </row>
+    <row r="92" spans="1:9">
+      <c s="4" r="C92" t="n"/>
+      <c s="4" r="D92" t="n"/>
+      <c s="4" r="G92" t="n"/>
+    </row>
+    <row r="93" spans="1:9">
+      <c s="4" r="C93" t="n"/>
+      <c s="4" r="D93" t="n"/>
+      <c s="4" r="G93" t="n"/>
+    </row>
+    <row r="94" spans="1:9">
+      <c s="3" r="C94" t="n"/>
+      <c s="3" r="D94" t="n"/>
+      <c s="3" r="G94" t="n"/>
+    </row>
+    <row r="95" spans="1:9">
+      <c s="4" r="C95" t="n"/>
+      <c s="4" r="D95" t="n"/>
+      <c s="3" r="G95" t="n"/>
+    </row>
+    <row r="96" spans="1:9">
+      <c s="4" r="C96" t="n"/>
+      <c s="4" r="D96" t="n"/>
+      <c s="3" r="G96" t="n"/>
+    </row>
+    <row r="97" spans="1:9">
+      <c s="4" r="C97" t="n"/>
+      <c s="4" r="D97" t="n"/>
+      <c s="4" r="G97" t="n"/>
+    </row>
+    <row r="98" spans="1:9">
+      <c s="4" r="C98" t="n"/>
+      <c s="4" r="D98" t="n"/>
+      <c s="3" r="G98" t="n"/>
+    </row>
+    <row r="99" spans="1:9">
+      <c s="4" r="C99" t="n"/>
+      <c s="4" r="D99" t="n"/>
+      <c s="4" r="G99" t="n"/>
+    </row>
+    <row r="100" spans="1:9">
+      <c s="4" r="C100" t="n"/>
+      <c s="4" r="D100" t="n"/>
+      <c s="4" r="G100" t="n"/>
+    </row>
+    <row r="101" spans="1:9">
+      <c s="3" r="C101" t="n"/>
+      <c s="3" r="D101" t="n"/>
+      <c s="4" r="G101" t="n"/>
+    </row>
+    <row r="102" spans="1:9">
+      <c s="3" r="C102" t="n"/>
+      <c s="3" r="D102" t="n"/>
+      <c s="4" r="G102" t="n"/>
+    </row>
+    <row r="103" spans="1:9">
+      <c s="3" r="C103" t="n"/>
+      <c s="3" r="D103" t="n"/>
+      <c s="3" r="G103" t="n"/>
+    </row>
+    <row r="104" spans="1:9">
+      <c s="4" r="C104" t="n"/>
+      <c s="4" r="D104" t="n"/>
+      <c s="4" r="G104" t="n"/>
+    </row>
+    <row r="105" spans="1:9">
+      <c s="4" r="C105" t="n"/>
+      <c s="4" r="D105" t="n"/>
+      <c s="4" r="G105" t="n"/>
+    </row>
+    <row r="106" spans="1:9">
+      <c s="3" r="C106" t="n"/>
+      <c s="3" r="D106" t="n"/>
+      <c s="3" r="G106" t="n"/>
+    </row>
+    <row r="107" spans="1:9">
+      <c s="4" r="C107" t="n"/>
+      <c s="4" r="D107" t="n"/>
+      <c s="3" r="G107" t="n"/>
+    </row>
+    <row r="108" spans="1:9">
+      <c s="4" r="C108" t="n"/>
+      <c s="4" r="D108" t="n"/>
+      <c s="4" r="G108" t="n"/>
+    </row>
+    <row r="109" spans="1:9">
+      <c s="4" r="C109" t="n"/>
+      <c s="4" r="D109" t="n"/>
+      <c s="4" r="G109" t="n"/>
+    </row>
+    <row r="110" spans="1:9">
+      <c s="3" r="C110" t="n"/>
+      <c s="3" r="D110" t="n"/>
+      <c s="4" r="G110" t="n"/>
+    </row>
+    <row r="111" spans="1:9">
+      <c s="4" r="C111" t="n"/>
+      <c s="4" r="D111" t="n"/>
+      <c s="4" r="G111" t="n"/>
+    </row>
+    <row r="112" spans="1:9">
+      <c s="3" r="C112" t="n"/>
+      <c s="3" r="D112" t="n"/>
+      <c s="4" r="G112" t="n"/>
+    </row>
+    <row r="113" spans="1:9">
+      <c s="4" r="C113" t="n"/>
+      <c s="4" r="D113" t="n"/>
+      <c s="3" r="G113" t="n"/>
+    </row>
+    <row r="114" spans="1:9">
+      <c s="4" r="C114" t="n"/>
+      <c s="4" r="D114" t="n"/>
+      <c s="4" r="G114" t="n"/>
+    </row>
+    <row r="115" spans="1:9">
+      <c s="4" r="C115" t="n"/>
+      <c s="4" r="D115" t="n"/>
+      <c s="3" r="G115" t="n"/>
+    </row>
+    <row r="116" spans="1:9">
+      <c s="3" r="C116" t="n"/>
+      <c s="3" r="D116" t="n"/>
+      <c s="4" r="G116" t="n"/>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
         <v>9</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B117" t="n">
         <v>12.74</v>
       </c>
-      <c s="8" r="C79" t="n">
+      <c s="8" r="C117" t="n">
         <v>1.66</v>
       </c>
-      <c s="8" r="D79" t="n">
+      <c s="8" r="D117" t="n">
         <v>13.03</v>
       </c>
-      <c r="E79" t="n">
+      <c r="E117" t="n">
         <v>2240</v>
       </c>
-      <c r="F79" t="n">
+      <c r="F117" t="n">
         <v>1400</v>
       </c>
-      <c s="8" r="G79" t="n">
+      <c s="8" r="G117" t="n">
         <v>0.62</v>
       </c>
-      <c r="H79" t="n">
+      <c r="H117" t="n">
         <v>3.95</v>
       </c>
-      <c r="I79" t="s">
+      <c r="I117" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="80" spans="1:9">
-      <c r="A80" t="s">
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>11</v>
+      </c>
+      <c r="B118" t="n">
+        <v>1998.1</v>
+      </c>
+      <c s="8" r="C118" t="n">
+        <v>65.28</v>
+      </c>
+      <c s="8" r="D118" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="E118" t="n">
+        <v>2791</v>
+      </c>
+      <c r="F118" t="n">
+        <v>2724</v>
+      </c>
+      <c s="8" r="G118" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="H118" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I118" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>17</v>
+      </c>
+      <c r="B119" t="n">
+        <v>62.13</v>
+      </c>
+      <c s="8" r="C119" t="n">
+        <v>10.63</v>
+      </c>
+      <c s="8" r="D119" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E119" t="n">
+        <v>2390</v>
+      </c>
+      <c r="F119" t="n">
+        <v>1583</v>
+      </c>
+      <c s="8" r="G119" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H119" t="s">
+        <v>18</v>
+      </c>
+      <c r="I119" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" t="n">
+        <v>222.98</v>
+      </c>
+      <c s="8" r="C120" t="n">
+        <v>3.28</v>
+      </c>
+      <c s="8" r="D120" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="E120" t="n">
+        <v>1715</v>
+      </c>
+      <c r="F120" t="n">
+        <v>1153</v>
+      </c>
+      <c s="8" r="G120" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H120" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I120" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
         <v>10</v>
       </c>
-      <c r="B80" t="n">
-        <v>1998.1</v>
-      </c>
-      <c s="8" r="C80" t="n">
-        <v>65.28</v>
-      </c>
-      <c s="8" r="D80" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="E80" t="n">
-        <v>2791</v>
-      </c>
-      <c r="F80" t="n">
-        <v>2724</v>
-      </c>
-      <c s="8" r="G80" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="H80" t="n">
-        <v>1.61</v>
-      </c>
-      <c r="I80" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81" t="s">
-        <v>11</v>
-      </c>
-      <c r="B81" t="n">
-        <v>62.13</v>
-      </c>
-      <c s="8" r="C81" t="n">
-        <v>10.63</v>
-      </c>
-      <c s="8" r="D81" t="n">
-        <v>17.11</v>
-      </c>
-      <c r="E81" t="n">
-        <v>2390</v>
-      </c>
-      <c r="F81" t="n">
-        <v>1583</v>
-      </c>
-      <c s="8" r="G81" t="n">
+      <c r="B121" t="n">
+        <v>25.2</v>
+      </c>
+      <c s="8" r="C121" t="n">
+        <v>0.15</v>
+      </c>
+      <c s="8" r="D121" t="n">
         <v>0.6</v>
       </c>
-      <c r="H81" t="s">
-        <v>12</v>
-      </c>
-      <c r="I81" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
-      <c r="A82" t="s">
-        <v>13</v>
-      </c>
-      <c r="B82" t="n">
-        <v>222.98</v>
-      </c>
-      <c s="8" r="C82" t="n">
-        <v>3.28</v>
-      </c>
-      <c s="8" r="D82" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="E82" t="n">
-        <v>1715</v>
-      </c>
-      <c r="F82" t="n">
-        <v>1153</v>
-      </c>
-      <c s="8" r="G82" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H82" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="I82" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
-      <c r="A83" t="s">
-        <v>14</v>
-      </c>
-      <c r="B83" t="n">
-        <v>25.2</v>
-      </c>
-      <c s="8" r="C83" t="n">
-        <v>0.15</v>
-      </c>
-      <c s="8" r="D83" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="E83" t="n">
+      <c r="E121" t="n">
         <v>2477</v>
       </c>
-      <c r="F83" t="n">
+      <c r="F121" t="n">
         <v>2465</v>
       </c>
-      <c s="8" r="G83" t="n">
+      <c s="8" r="G121" t="n">
         <v>0.5</v>
       </c>
-      <c r="H83" t="n">
+      <c r="H121" t="n">
         <v>3.6</v>
       </c>
-      <c r="I83" t="s">
+      <c r="I121" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2235,4 +3469,87 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c s="12" r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c s="13" r="B2" t="n"/>
+      <c s="14" r="C2" t="n"/>
+      <c s="15" r="D2" t="n"/>
+      <c s="16" r="E2" t="n"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c s="12" r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c s="13" r="B3" t="n"/>
+      <c s="15" r="C3" t="n"/>
+      <c s="14" r="E3" t="n"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c s="16" r="C4" t="n"/>
+      <c s="15" r="D4" t="n"/>
+      <c s="15" r="E4" t="n"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c s="12" r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c s="16" r="D5" t="n"/>
+      <c s="14" r="E5" t="n"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated tab price,50ma,200 tabs.  still need data
</commit_message>
<xml_diff>
--- a/Stock_Parser/demo.xlsx
+++ b/Stock_Parser/demo.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8970" windowWidth="21570" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8970" windowWidth="21570" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Daily Stock List" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cumulative_Stock_List" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Price Changes" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="50 Day MA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="200 Day MA" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -16,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>Stock Additions</t>
   </si>
@@ -48,13 +50,13 @@
     <t>CRON</t>
   </si>
   <si>
-    <t>AMD</t>
-  </si>
-  <si>
     <t>AMZN</t>
   </si>
   <si>
     <t>AAPL</t>
+  </si>
+  <si>
+    <t>AMD</t>
   </si>
   <si>
     <t>CRM</t>
@@ -144,6 +146,9 @@
     <t>8/30/2018</t>
   </si>
   <si>
+    <t>Stock/Date</t>
+  </si>
+  <si>
     <t>Goog</t>
   </si>
 </sst>
@@ -152,7 +157,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="20">
+  <fonts count="26">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -250,24 +255,48 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FF00"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FF00"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FF00"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <color rgb="00FF0000"/>
     </font>
     <font>
       <color rgb="0000FF00"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -282,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -296,16 +325,20 @@
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="16" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="19" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -625,22 +658,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>11.31</v>
-      </c>
-      <c s="21" r="C4" t="n">
-        <v>-1.43</v>
-      </c>
-      <c s="21" r="D4" t="n">
-        <v>-12.64</v>
+        <v>11.96</v>
+      </c>
+      <c s="25" r="C4" t="n">
+        <v>-0.79</v>
+      </c>
+      <c s="25" r="D4" t="n">
+        <v>-6.61</v>
       </c>
       <c r="E4" t="n">
-        <v>804</v>
+        <v>1266</v>
       </c>
       <c r="F4" t="n">
-        <v>395</v>
-      </c>
-      <c s="22" r="G4" t="n">
-        <v>0.67</v>
+        <v>690</v>
+      </c>
+      <c s="26" r="G4" t="n">
+        <v>0.65</v>
       </c>
       <c r="H4" t="n">
         <v>3.95</v>
@@ -651,25 +684,25 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>25.25</v>
-      </c>
-      <c s="22" r="C5" t="n">
-        <v>0.05</v>
-      </c>
-      <c s="22" r="D5" t="n">
-        <v>0.2</v>
+        <v>2019.83</v>
+      </c>
+      <c s="26" r="C5" t="n">
+        <v>21.73</v>
+      </c>
+      <c s="26" r="D5" t="n">
+        <v>1.08</v>
       </c>
       <c r="E5" t="n">
-        <v>537</v>
+        <v>1526</v>
       </c>
       <c r="F5" t="n">
-        <v>375</v>
-      </c>
-      <c s="22" r="G5" t="n">
-        <v>0.59</v>
+        <v>1176</v>
+      </c>
+      <c s="26" r="G5" t="n">
+        <v>0.5600000000000001</v>
       </c>
       <c r="H5" t="n">
-        <v>3.6</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -677,25 +710,25 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>2001.13</v>
-      </c>
-      <c s="22" r="C6" t="n">
-        <v>3.03</v>
-      </c>
-      <c s="22" r="D6" t="n">
-        <v>0.15</v>
+        <v>224.41</v>
+      </c>
+      <c s="26" r="C6" t="n">
+        <v>1.43</v>
+      </c>
+      <c s="26" r="D6" t="n">
+        <v>0.64</v>
       </c>
       <c r="E6" t="n">
-        <v>865</v>
+        <v>970</v>
       </c>
       <c r="F6" t="n">
-        <v>711</v>
-      </c>
-      <c s="22" r="G6" t="n">
-        <v>0.55</v>
+        <v>546</v>
+      </c>
+      <c s="26" r="G6" t="n">
+        <v>0.64</v>
       </c>
       <c r="H6" t="n">
-        <v>1.61</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -703,25 +736,25 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>222.97</v>
-      </c>
-      <c s="21" r="C7" t="n">
-        <v>-0.01</v>
-      </c>
-      <c s="22" r="D7" t="n">
-        <v>-0</v>
+        <v>25.33</v>
+      </c>
+      <c s="26" r="C7" t="n">
+        <v>0.13</v>
+      </c>
+      <c s="26" r="D7" t="n">
+        <v>0.51</v>
       </c>
       <c r="E7" t="n">
-        <v>656</v>
+        <v>913</v>
       </c>
       <c r="F7" t="n">
-        <v>394</v>
-      </c>
-      <c s="22" r="G7" t="n">
-        <v>0.62</v>
+        <v>727</v>
+      </c>
+      <c s="26" r="G7" t="n">
+        <v>0.5600000000000001</v>
       </c>
       <c r="H7" t="n">
-        <v>1.14</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -729,22 +762,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>150.19</v>
-      </c>
-      <c s="21" r="C8" t="n">
-        <v>-4.61</v>
-      </c>
-      <c s="21" r="D8" t="n">
-        <v>-3.07</v>
+        <v>151.82</v>
+      </c>
+      <c s="25" r="C8" t="n">
+        <v>-2.98</v>
+      </c>
+      <c s="25" r="D8" t="n">
+        <v>-1.96</v>
       </c>
       <c r="E8" t="n">
-        <v>916</v>
+        <v>1112</v>
       </c>
       <c r="F8" t="n">
-        <v>660</v>
-      </c>
-      <c s="22" r="G8" t="n">
-        <v>0.58</v>
+        <v>787</v>
+      </c>
+      <c s="26" r="G8" t="n">
+        <v>0.59</v>
       </c>
       <c r="H8" t="n">
         <v>1.13</v>
@@ -752,7 +785,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="n">
         <v>222.98</v>
@@ -1090,7 +1123,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B22" t="n">
         <v>25.2</v>
@@ -1246,7 +1279,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28" t="n">
         <v>1998.1</v>
@@ -1412,7 +1445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="H13" sqref="H13"/>
@@ -1775,10 +1808,10 @@
       <c r="B13" t="n">
         <v>11.42</v>
       </c>
-      <c s="17" r="C13" t="n">
+      <c s="13" r="C13" t="n">
         <v>-1.32</v>
       </c>
-      <c s="17" r="D13" t="n">
+      <c s="13" r="D13" t="n">
         <v>-11.56</v>
       </c>
       <c r="E13" t="n">
@@ -1787,7 +1820,7 @@
       <c r="F13" t="n">
         <v>395</v>
       </c>
-      <c s="18" r="G13" t="n">
+      <c s="14" r="G13" t="n">
         <v>0.67</v>
       </c>
       <c r="H13" t="n">
@@ -1804,10 +1837,10 @@
       <c r="B14" t="n">
         <v>11.39</v>
       </c>
-      <c s="19" r="C14" t="n">
+      <c s="15" r="C14" t="n">
         <v>-1.35</v>
       </c>
-      <c s="19" r="D14" t="n">
+      <c s="15" r="D14" t="n">
         <v>-11.85</v>
       </c>
       <c r="E14" t="n">
@@ -1816,7 +1849,7 @@
       <c r="F14" t="n">
         <v>395</v>
       </c>
-      <c s="20" r="G14" t="n">
+      <c s="16" r="G14" t="n">
         <v>0.67</v>
       </c>
       <c r="H14" t="n">
@@ -1833,10 +1866,10 @@
       <c r="B15" t="n">
         <v>11.31</v>
       </c>
-      <c s="21" r="C15" t="n">
+      <c s="17" r="C15" t="n">
         <v>-1.43</v>
       </c>
-      <c s="21" r="D15" t="n">
+      <c s="17" r="D15" t="n">
         <v>-12.64</v>
       </c>
       <c r="E15" t="n">
@@ -1845,7 +1878,7 @@
       <c r="F15" t="n">
         <v>395</v>
       </c>
-      <c s="22" r="G15" t="n">
+      <c s="18" r="G15" t="n">
         <v>0.67</v>
       </c>
       <c r="H15" t="n">
@@ -1857,86 +1890,86 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B16" t="n">
-        <v>1998.1</v>
-      </c>
-      <c s="8" r="C16" t="n">
-        <v>65.28</v>
-      </c>
-      <c s="8" r="D16" t="n">
-        <v>3.27</v>
+        <v>11.46</v>
+      </c>
+      <c s="21" r="C16" t="n">
+        <v>-1.28</v>
+      </c>
+      <c s="21" r="D16" t="n">
+        <v>-11.17</v>
       </c>
       <c r="E16" t="n">
-        <v>2791</v>
+        <v>1069</v>
       </c>
       <c r="F16" t="n">
-        <v>2724</v>
-      </c>
-      <c s="8" r="G16" t="n">
-        <v>0.51</v>
+        <v>554</v>
+      </c>
+      <c s="22" r="G16" t="n">
+        <v>0.66</v>
       </c>
       <c r="H16" t="n">
-        <v>1.61</v>
+        <v>3.95</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" t="n">
-        <v>1998.1</v>
-      </c>
-      <c s="8" r="C17" t="n">
-        <v>65.28</v>
-      </c>
-      <c s="8" r="D17" t="n">
-        <v>3.27</v>
+        <v>11.64</v>
+      </c>
+      <c s="23" r="C17" t="n">
+        <v>-1.1</v>
+      </c>
+      <c s="23" r="D17" t="n">
+        <v>-9.449999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>2791</v>
+        <v>1069</v>
       </c>
       <c r="F17" t="n">
-        <v>2724</v>
-      </c>
-      <c s="8" r="G17" t="n">
-        <v>0.51</v>
+        <v>554</v>
+      </c>
+      <c s="24" r="G17" t="n">
+        <v>0.66</v>
       </c>
       <c r="H17" t="n">
-        <v>1.61</v>
+        <v>3.95</v>
       </c>
       <c r="I17" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18" t="n">
-        <v>2005.03</v>
-      </c>
-      <c s="8" r="C18" t="n">
-        <v>6.93</v>
-      </c>
-      <c s="8" r="D18" t="n">
-        <v>0.35</v>
+        <v>11.69</v>
+      </c>
+      <c s="23" r="C18" t="n">
+        <v>-1.05</v>
+      </c>
+      <c s="23" r="D18" t="n">
+        <v>-8.98</v>
       </c>
       <c r="E18" t="n">
-        <v>322</v>
+        <v>1069</v>
       </c>
       <c r="F18" t="n">
-        <v>320</v>
-      </c>
-      <c s="8" r="G18" t="n">
-        <v>0.5</v>
+        <v>554</v>
+      </c>
+      <c s="24" r="G18" t="n">
+        <v>0.66</v>
       </c>
       <c r="H18" t="n">
-        <v>1.61</v>
+        <v>3.95</v>
       </c>
       <c r="I18" t="s">
         <v>41</v>
@@ -1944,28 +1977,28 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" t="n">
-        <v>1999.03</v>
-      </c>
-      <c s="11" r="C19" t="n">
-        <v>0.93</v>
-      </c>
-      <c s="11" r="D19" t="n">
-        <v>0.05</v>
+        <v>11.9</v>
+      </c>
+      <c s="23" r="C19" t="n">
+        <v>-0.84</v>
+      </c>
+      <c s="23" r="D19" t="n">
+        <v>-7.06</v>
       </c>
       <c r="E19" t="n">
-        <v>740</v>
+        <v>1266</v>
       </c>
       <c r="F19" t="n">
-        <v>607</v>
-      </c>
-      <c s="11" r="G19" t="n">
-        <v>0.55</v>
+        <v>690</v>
+      </c>
+      <c s="24" r="G19" t="n">
+        <v>0.65</v>
       </c>
       <c r="H19" t="n">
-        <v>1.61</v>
+        <v>3.95</v>
       </c>
       <c r="I19" t="s">
         <v>41</v>
@@ -1973,28 +2006,28 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" t="n">
-        <v>1997.49</v>
-      </c>
-      <c s="10" r="C20" t="n">
-        <v>-0.61</v>
-      </c>
-      <c s="10" r="D20" t="n">
-        <v>-0.03</v>
+        <v>11.94</v>
+      </c>
+      <c s="23" r="C20" t="n">
+        <v>-0.8</v>
+      </c>
+      <c s="23" r="D20" t="n">
+        <v>-6.7</v>
       </c>
       <c r="E20" t="n">
-        <v>740</v>
+        <v>1266</v>
       </c>
       <c r="F20" t="n">
-        <v>607</v>
-      </c>
-      <c s="11" r="G20" t="n">
-        <v>0.55</v>
+        <v>690</v>
+      </c>
+      <c s="24" r="G20" t="n">
+        <v>0.65</v>
       </c>
       <c r="H20" t="n">
-        <v>1.61</v>
+        <v>3.95</v>
       </c>
       <c r="I20" t="s">
         <v>41</v>
@@ -2002,28 +2035,28 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21" t="n">
-        <v>1997.93</v>
-      </c>
-      <c s="10" r="C21" t="n">
-        <v>-0.17</v>
-      </c>
-      <c s="10" r="D21" t="n">
-        <v>-0.01</v>
+        <v>11.96</v>
+      </c>
+      <c s="25" r="C21" t="n">
+        <v>-0.79</v>
+      </c>
+      <c s="25" r="D21" t="n">
+        <v>-6.61</v>
       </c>
       <c r="E21" t="n">
-        <v>740</v>
+        <v>1266</v>
       </c>
       <c r="F21" t="n">
-        <v>607</v>
-      </c>
-      <c s="11" r="G21" t="n">
-        <v>0.55</v>
+        <v>690</v>
+      </c>
+      <c s="26" r="G21" t="n">
+        <v>0.65</v>
       </c>
       <c r="H21" t="n">
-        <v>1.61</v>
+        <v>3.95</v>
       </c>
       <c r="I21" t="s">
         <v>41</v>
@@ -2031,83 +2064,83 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" t="n">
-        <v>1999.18</v>
-      </c>
-      <c s="11" r="C22" t="n">
-        <v>1.08</v>
-      </c>
-      <c s="11" r="D22" t="n">
-        <v>0.05</v>
+        <v>1998.1</v>
+      </c>
+      <c s="8" r="C22" t="n">
+        <v>65.28</v>
+      </c>
+      <c s="8" r="D22" t="n">
+        <v>3.27</v>
       </c>
       <c r="E22" t="n">
-        <v>740</v>
+        <v>2791</v>
       </c>
       <c r="F22" t="n">
-        <v>607</v>
-      </c>
-      <c s="11" r="G22" t="n">
-        <v>0.55</v>
+        <v>2724</v>
+      </c>
+      <c s="8" r="G22" t="n">
+        <v>0.51</v>
       </c>
       <c r="H22" t="n">
         <v>1.61</v>
       </c>
       <c r="I22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" t="n">
-        <v>2002.77</v>
-      </c>
-      <c s="18" r="C23" t="n">
-        <v>4.67</v>
-      </c>
-      <c s="18" r="D23" t="n">
-        <v>0.23</v>
+        <v>1998.1</v>
+      </c>
+      <c s="8" r="C23" t="n">
+        <v>65.28</v>
+      </c>
+      <c s="8" r="D23" t="n">
+        <v>3.27</v>
       </c>
       <c r="E23" t="n">
-        <v>865</v>
+        <v>2791</v>
       </c>
       <c r="F23" t="n">
-        <v>711</v>
-      </c>
-      <c s="18" r="G23" t="n">
-        <v>0.55</v>
+        <v>2724</v>
+      </c>
+      <c s="8" r="G23" t="n">
+        <v>0.51</v>
       </c>
       <c r="H23" t="n">
         <v>1.61</v>
       </c>
       <c r="I23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" t="n">
-        <v>2002.22</v>
-      </c>
-      <c s="20" r="C24" t="n">
-        <v>4.12</v>
-      </c>
-      <c s="20" r="D24" t="n">
-        <v>0.21</v>
+        <v>2005.03</v>
+      </c>
+      <c s="8" r="C24" t="n">
+        <v>6.93</v>
+      </c>
+      <c s="8" r="D24" t="n">
+        <v>0.35</v>
       </c>
       <c r="E24" t="n">
-        <v>865</v>
+        <v>322</v>
       </c>
       <c r="F24" t="n">
-        <v>711</v>
-      </c>
-      <c s="20" r="G24" t="n">
-        <v>0.55</v>
+        <v>320</v>
+      </c>
+      <c s="8" r="G24" t="n">
+        <v>0.5</v>
       </c>
       <c r="H24" t="n">
         <v>1.61</v>
@@ -2118,24 +2151,24 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25" t="n">
-        <v>2001.13</v>
-      </c>
-      <c s="22" r="C25" t="n">
-        <v>3.03</v>
-      </c>
-      <c s="22" r="D25" t="n">
-        <v>0.15</v>
+        <v>1999.03</v>
+      </c>
+      <c s="11" r="C25" t="n">
+        <v>0.93</v>
+      </c>
+      <c s="11" r="D25" t="n">
+        <v>0.05</v>
       </c>
       <c r="E25" t="n">
-        <v>865</v>
+        <v>740</v>
       </c>
       <c r="F25" t="n">
-        <v>711</v>
-      </c>
-      <c s="22" r="G25" t="n">
+        <v>607</v>
+      </c>
+      <c s="11" r="G25" t="n">
         <v>0.55</v>
       </c>
       <c r="H25" t="n">
@@ -2147,144 +2180,144 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B26" t="n">
-        <v>62.13</v>
-      </c>
-      <c s="8" r="C26" t="n">
-        <v>10.63</v>
-      </c>
-      <c s="8" r="D26" t="n">
-        <v>17.11</v>
+        <v>1997.49</v>
+      </c>
+      <c s="10" r="C26" t="n">
+        <v>-0.61</v>
+      </c>
+      <c s="10" r="D26" t="n">
+        <v>-0.03</v>
       </c>
       <c r="E26" t="n">
-        <v>2390</v>
+        <v>740</v>
       </c>
       <c r="F26" t="n">
-        <v>1583</v>
-      </c>
-      <c s="8" r="G26" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H26" t="s">
-        <v>18</v>
+        <v>607</v>
+      </c>
+      <c s="11" r="G26" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1.61</v>
       </c>
       <c r="I26" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B27" t="n">
-        <v>62.13</v>
-      </c>
-      <c s="8" r="C27" t="n">
-        <v>10.63</v>
-      </c>
-      <c s="8" r="D27" t="n">
-        <v>17.11</v>
+        <v>1997.93</v>
+      </c>
+      <c s="10" r="C27" t="n">
+        <v>-0.17</v>
+      </c>
+      <c s="10" r="D27" t="n">
+        <v>-0.01</v>
       </c>
       <c r="E27" t="n">
-        <v>2390</v>
+        <v>740</v>
       </c>
       <c r="F27" t="n">
-        <v>1583</v>
-      </c>
-      <c s="8" r="G27" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H27" t="s">
-        <v>18</v>
+        <v>607</v>
+      </c>
+      <c s="11" r="G27" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1.61</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" t="n">
-        <v>222.98</v>
-      </c>
-      <c s="8" r="C28" t="n">
-        <v>3.28</v>
-      </c>
-      <c s="8" r="D28" t="n">
-        <v>1.47</v>
+        <v>1999.18</v>
+      </c>
+      <c s="11" r="C28" t="n">
+        <v>1.08</v>
+      </c>
+      <c s="11" r="D28" t="n">
+        <v>0.05</v>
       </c>
       <c r="E28" t="n">
-        <v>1715</v>
+        <v>740</v>
       </c>
       <c r="F28" t="n">
-        <v>1153</v>
-      </c>
-      <c s="8" r="G28" t="n">
-        <v>0.6</v>
+        <v>607</v>
+      </c>
+      <c s="11" r="G28" t="n">
+        <v>0.55</v>
       </c>
       <c r="H28" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I28" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" t="n">
-        <v>222.98</v>
-      </c>
-      <c s="8" r="C29" t="n">
-        <v>3.28</v>
-      </c>
-      <c s="8" r="D29" t="n">
-        <v>1.47</v>
+        <v>2002.77</v>
+      </c>
+      <c s="14" r="C29" t="n">
+        <v>4.67</v>
+      </c>
+      <c s="14" r="D29" t="n">
+        <v>0.23</v>
       </c>
       <c r="E29" t="n">
-        <v>1715</v>
+        <v>865</v>
       </c>
       <c r="F29" t="n">
-        <v>1153</v>
-      </c>
-      <c s="8" r="G29" t="n">
-        <v>0.6</v>
+        <v>711</v>
+      </c>
+      <c s="14" r="G29" t="n">
+        <v>0.55</v>
       </c>
       <c r="H29" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I29" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" t="n">
-        <v>224.43</v>
-      </c>
-      <c s="8" r="C30" t="n">
-        <v>1.45</v>
-      </c>
-      <c s="8" r="D30" t="n">
-        <v>0.65</v>
+        <v>2002.22</v>
+      </c>
+      <c s="16" r="C30" t="n">
+        <v>4.12</v>
+      </c>
+      <c s="16" r="D30" t="n">
+        <v>0.21</v>
       </c>
       <c r="E30" t="n">
-        <v>272</v>
+        <v>865</v>
       </c>
       <c r="F30" t="n">
-        <v>186</v>
-      </c>
-      <c s="8" r="G30" t="n">
-        <v>0.59</v>
+        <v>711</v>
+      </c>
+      <c s="16" r="G30" t="n">
+        <v>0.55</v>
       </c>
       <c r="H30" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I30" t="s">
         <v>41</v>
@@ -2292,28 +2325,28 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" t="n">
-        <v>222.76</v>
-      </c>
-      <c s="10" r="C31" t="n">
-        <v>-0.22</v>
-      </c>
-      <c s="10" r="D31" t="n">
-        <v>-0.1</v>
+        <v>2001.13</v>
+      </c>
+      <c s="18" r="C31" t="n">
+        <v>3.03</v>
+      </c>
+      <c s="18" r="D31" t="n">
+        <v>0.15</v>
       </c>
       <c r="E31" t="n">
-        <v>568</v>
+        <v>865</v>
       </c>
       <c r="F31" t="n">
-        <v>345</v>
-      </c>
-      <c s="11" r="G31" t="n">
-        <v>0.62</v>
+        <v>711</v>
+      </c>
+      <c s="18" r="G31" t="n">
+        <v>0.55</v>
       </c>
       <c r="H31" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I31" t="s">
         <v>41</v>
@@ -2321,28 +2354,28 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" t="n">
-        <v>222.8</v>
-      </c>
-      <c s="10" r="C32" t="n">
-        <v>-0.18</v>
-      </c>
-      <c s="10" r="D32" t="n">
-        <v>-0.08</v>
+        <v>2016.01</v>
+      </c>
+      <c s="22" r="C32" t="n">
+        <v>17.91</v>
+      </c>
+      <c s="22" r="D32" t="n">
+        <v>0.89</v>
       </c>
       <c r="E32" t="n">
-        <v>568</v>
+        <v>1152</v>
       </c>
       <c r="F32" t="n">
-        <v>345</v>
-      </c>
-      <c s="11" r="G32" t="n">
-        <v>0.62</v>
+        <v>877</v>
+      </c>
+      <c s="22" r="G32" t="n">
+        <v>0.57</v>
       </c>
       <c r="H32" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I32" t="s">
         <v>41</v>
@@ -2350,28 +2383,28 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33" t="n">
-        <v>222.76</v>
-      </c>
-      <c s="10" r="C33" t="n">
-        <v>-0.22</v>
-      </c>
-      <c s="10" r="D33" t="n">
-        <v>-0.1</v>
+        <v>2016.85</v>
+      </c>
+      <c s="24" r="C33" t="n">
+        <v>18.75</v>
+      </c>
+      <c s="24" r="D33" t="n">
+        <v>0.93</v>
       </c>
       <c r="E33" t="n">
-        <v>568</v>
+        <v>1152</v>
       </c>
       <c r="F33" t="n">
-        <v>345</v>
-      </c>
-      <c s="11" r="G33" t="n">
-        <v>0.62</v>
+        <v>877</v>
+      </c>
+      <c s="24" r="G33" t="n">
+        <v>0.57</v>
       </c>
       <c r="H33" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I33" t="s">
         <v>41</v>
@@ -2379,28 +2412,28 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34" t="n">
-        <v>222.43</v>
-      </c>
-      <c s="10" r="C34" t="n">
-        <v>-0.55</v>
-      </c>
-      <c s="10" r="D34" t="n">
-        <v>-0.25</v>
+        <v>2017.24</v>
+      </c>
+      <c s="24" r="C34" t="n">
+        <v>19.14</v>
+      </c>
+      <c s="24" r="D34" t="n">
+        <v>0.95</v>
       </c>
       <c r="E34" t="n">
-        <v>568</v>
+        <v>1152</v>
       </c>
       <c r="F34" t="n">
-        <v>345</v>
-      </c>
-      <c s="11" r="G34" t="n">
-        <v>0.62</v>
+        <v>877</v>
+      </c>
+      <c s="24" r="G34" t="n">
+        <v>0.57</v>
       </c>
       <c r="H34" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I34" t="s">
         <v>41</v>
@@ -2408,28 +2441,28 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B35" t="n">
-        <v>223.03</v>
-      </c>
-      <c s="18" r="C35" t="n">
-        <v>0.05</v>
-      </c>
-      <c s="18" r="D35" t="n">
-        <v>0.02</v>
+        <v>2018.63</v>
+      </c>
+      <c s="24" r="C35" t="n">
+        <v>20.53</v>
+      </c>
+      <c s="24" r="D35" t="n">
+        <v>1.02</v>
       </c>
       <c r="E35" t="n">
-        <v>656</v>
+        <v>1526</v>
       </c>
       <c r="F35" t="n">
-        <v>394</v>
-      </c>
-      <c s="18" r="G35" t="n">
-        <v>0.62</v>
+        <v>1176</v>
+      </c>
+      <c s="24" r="G35" t="n">
+        <v>0.5600000000000001</v>
       </c>
       <c r="H35" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I35" t="s">
         <v>41</v>
@@ -2437,28 +2470,28 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" t="n">
-        <v>222.91</v>
-      </c>
-      <c s="19" r="C36" t="n">
-        <v>-0.07000000000000001</v>
-      </c>
-      <c s="19" r="D36" t="n">
-        <v>-0.03</v>
+        <v>2016.54</v>
+      </c>
+      <c s="24" r="C36" t="n">
+        <v>18.44</v>
+      </c>
+      <c s="24" r="D36" t="n">
+        <v>0.91</v>
       </c>
       <c r="E36" t="n">
-        <v>656</v>
+        <v>1526</v>
       </c>
       <c r="F36" t="n">
-        <v>394</v>
-      </c>
-      <c s="20" r="G36" t="n">
-        <v>0.62</v>
+        <v>1176</v>
+      </c>
+      <c s="24" r="G36" t="n">
+        <v>0.5600000000000001</v>
       </c>
       <c r="H36" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I36" t="s">
         <v>41</v>
@@ -2466,28 +2499,28 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B37" t="n">
-        <v>222.97</v>
-      </c>
-      <c s="21" r="C37" t="n">
-        <v>-0.01</v>
-      </c>
-      <c s="22" r="D37" t="n">
-        <v>-0</v>
+        <v>2019.83</v>
+      </c>
+      <c s="26" r="C37" t="n">
+        <v>21.73</v>
+      </c>
+      <c s="26" r="D37" t="n">
+        <v>1.08</v>
       </c>
       <c r="E37" t="n">
-        <v>656</v>
+        <v>1526</v>
       </c>
       <c r="F37" t="n">
-        <v>394</v>
-      </c>
-      <c s="22" r="G37" t="n">
-        <v>0.62</v>
+        <v>1176</v>
+      </c>
+      <c s="26" r="G37" t="n">
+        <v>0.5600000000000001</v>
       </c>
       <c r="H37" t="n">
-        <v>1.14</v>
+        <v>1.61</v>
       </c>
       <c r="I37" t="s">
         <v>41</v>
@@ -2495,28 +2528,28 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B38" t="n">
-        <v>25.2</v>
+        <v>62.13</v>
       </c>
       <c s="8" r="C38" t="n">
-        <v>0.15</v>
+        <v>10.63</v>
       </c>
       <c s="8" r="D38" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2390</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1583</v>
+      </c>
+      <c s="8" r="G38" t="n">
         <v>0.6</v>
       </c>
-      <c r="E38" t="n">
-        <v>2477</v>
-      </c>
-      <c r="F38" t="n">
-        <v>2465</v>
-      </c>
-      <c s="8" r="G38" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H38" t="n">
-        <v>3.6</v>
+      <c r="H38" t="s">
+        <v>18</v>
       </c>
       <c r="I38" t="s">
         <v>37</v>
@@ -2524,28 +2557,28 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B39" t="n">
-        <v>25.2</v>
+        <v>62.13</v>
       </c>
       <c s="8" r="C39" t="n">
-        <v>0.15</v>
+        <v>10.63</v>
       </c>
       <c s="8" r="D39" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2390</v>
+      </c>
+      <c r="F39" t="n">
+        <v>1583</v>
+      </c>
+      <c s="8" r="G39" t="n">
         <v>0.6</v>
       </c>
-      <c r="E39" t="n">
-        <v>2477</v>
-      </c>
-      <c r="F39" t="n">
-        <v>2465</v>
-      </c>
-      <c s="8" r="G39" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H39" t="n">
-        <v>3.6</v>
+      <c r="H39" t="s">
+        <v>18</v>
       </c>
       <c r="I39" t="s">
         <v>37</v>
@@ -2553,86 +2586,86 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B40" t="n">
-        <v>24.98</v>
-      </c>
-      <c s="10" r="C40" t="n">
-        <v>-0.22</v>
-      </c>
-      <c s="10" r="D40" t="n">
-        <v>-0.88</v>
+        <v>222.98</v>
+      </c>
+      <c s="8" r="C40" t="n">
+        <v>3.28</v>
+      </c>
+      <c s="8" r="D40" t="n">
+        <v>1.47</v>
       </c>
       <c r="E40" t="n">
-        <v>449</v>
+        <v>1715</v>
       </c>
       <c r="F40" t="n">
-        <v>306</v>
-      </c>
-      <c s="11" r="G40" t="n">
-        <v>0.59</v>
+        <v>1153</v>
+      </c>
+      <c s="8" r="G40" t="n">
+        <v>0.6</v>
       </c>
       <c r="H40" t="n">
-        <v>3.6</v>
+        <v>1.14</v>
       </c>
       <c r="I40" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B41" t="n">
-        <v>24.99</v>
-      </c>
-      <c s="10" r="C41" t="n">
-        <v>-0.21</v>
-      </c>
-      <c s="10" r="D41" t="n">
-        <v>-0.84</v>
+        <v>222.98</v>
+      </c>
+      <c s="8" r="C41" t="n">
+        <v>3.28</v>
+      </c>
+      <c s="8" r="D41" t="n">
+        <v>1.47</v>
       </c>
       <c r="E41" t="n">
-        <v>449</v>
+        <v>1715</v>
       </c>
       <c r="F41" t="n">
-        <v>306</v>
-      </c>
-      <c s="11" r="G41" t="n">
-        <v>0.59</v>
+        <v>1153</v>
+      </c>
+      <c s="8" r="G41" t="n">
+        <v>0.6</v>
       </c>
       <c r="H41" t="n">
-        <v>3.6</v>
+        <v>1.14</v>
       </c>
       <c r="I41" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B42" t="n">
-        <v>25.04</v>
-      </c>
-      <c s="10" r="C42" t="n">
-        <v>-0.16</v>
-      </c>
-      <c s="10" r="D42" t="n">
-        <v>-0.64</v>
+        <v>224.43</v>
+      </c>
+      <c s="8" r="C42" t="n">
+        <v>1.45</v>
+      </c>
+      <c s="8" r="D42" t="n">
+        <v>0.65</v>
       </c>
       <c r="E42" t="n">
-        <v>449</v>
+        <v>272</v>
       </c>
       <c r="F42" t="n">
-        <v>306</v>
-      </c>
-      <c s="11" r="G42" t="n">
+        <v>186</v>
+      </c>
+      <c s="8" r="G42" t="n">
         <v>0.59</v>
       </c>
       <c r="H42" t="n">
-        <v>3.6</v>
+        <v>1.14</v>
       </c>
       <c r="I42" t="s">
         <v>41</v>
@@ -2640,28 +2673,28 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B43" t="n">
-        <v>25.1</v>
+        <v>222.76</v>
       </c>
       <c s="10" r="C43" t="n">
+        <v>-0.22</v>
+      </c>
+      <c s="10" r="D43" t="n">
         <v>-0.1</v>
       </c>
-      <c s="10" r="D43" t="n">
-        <v>-0.4</v>
-      </c>
       <c r="E43" t="n">
-        <v>449</v>
+        <v>568</v>
       </c>
       <c r="F43" t="n">
-        <v>306</v>
+        <v>345</v>
       </c>
       <c s="11" r="G43" t="n">
-        <v>0.59</v>
+        <v>0.62</v>
       </c>
       <c r="H43" t="n">
-        <v>3.6</v>
+        <v>1.14</v>
       </c>
       <c r="I43" t="s">
         <v>41</v>
@@ -2669,28 +2702,28 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B44" t="n">
-        <v>25.25</v>
-      </c>
-      <c s="18" r="C44" t="n">
-        <v>0.05</v>
-      </c>
-      <c s="18" r="D44" t="n">
-        <v>0.2</v>
+        <v>222.8</v>
+      </c>
+      <c s="10" r="C44" t="n">
+        <v>-0.18</v>
+      </c>
+      <c s="10" r="D44" t="n">
+        <v>-0.08</v>
       </c>
       <c r="E44" t="n">
-        <v>537</v>
+        <v>568</v>
       </c>
       <c r="F44" t="n">
-        <v>375</v>
-      </c>
-      <c s="18" r="G44" t="n">
-        <v>0.59</v>
+        <v>345</v>
+      </c>
+      <c s="11" r="G44" t="n">
+        <v>0.62</v>
       </c>
       <c r="H44" t="n">
-        <v>3.6</v>
+        <v>1.14</v>
       </c>
       <c r="I44" t="s">
         <v>41</v>
@@ -2698,28 +2731,28 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B45" t="n">
-        <v>25.33</v>
-      </c>
-      <c s="20" r="C45" t="n">
-        <v>0.13</v>
-      </c>
-      <c s="20" r="D45" t="n">
-        <v>0.51</v>
+        <v>222.76</v>
+      </c>
+      <c s="10" r="C45" t="n">
+        <v>-0.22</v>
+      </c>
+      <c s="10" r="D45" t="n">
+        <v>-0.1</v>
       </c>
       <c r="E45" t="n">
-        <v>537</v>
+        <v>568</v>
       </c>
       <c r="F45" t="n">
-        <v>375</v>
-      </c>
-      <c s="20" r="G45" t="n">
-        <v>0.59</v>
+        <v>345</v>
+      </c>
+      <c s="11" r="G45" t="n">
+        <v>0.62</v>
       </c>
       <c r="H45" t="n">
-        <v>3.6</v>
+        <v>1.14</v>
       </c>
       <c r="I45" t="s">
         <v>41</v>
@@ -2727,28 +2760,28 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B46" t="n">
-        <v>25.25</v>
-      </c>
-      <c s="22" r="C46" t="n">
-        <v>0.05</v>
-      </c>
-      <c s="22" r="D46" t="n">
-        <v>0.2</v>
+        <v>222.43</v>
+      </c>
+      <c s="10" r="C46" t="n">
+        <v>-0.55</v>
+      </c>
+      <c s="10" r="D46" t="n">
+        <v>-0.25</v>
       </c>
       <c r="E46" t="n">
-        <v>537</v>
+        <v>568</v>
       </c>
       <c r="F46" t="n">
-        <v>375</v>
-      </c>
-      <c s="22" r="G46" t="n">
-        <v>0.59</v>
+        <v>345</v>
+      </c>
+      <c s="11" r="G46" t="n">
+        <v>0.62</v>
       </c>
       <c r="H46" t="n">
-        <v>3.6</v>
+        <v>1.14</v>
       </c>
       <c r="I46" t="s">
         <v>41</v>
@@ -2756,28 +2789,28 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B47" t="n">
-        <v>44.69</v>
-      </c>
-      <c s="9" r="C47" t="n">
-        <v>-1.71</v>
-      </c>
-      <c s="9" r="D47" t="n">
-        <v>-3.83</v>
+        <v>223.03</v>
+      </c>
+      <c s="14" r="C47" t="n">
+        <v>0.05</v>
+      </c>
+      <c s="14" r="D47" t="n">
+        <v>0.02</v>
       </c>
       <c r="E47" t="n">
-        <v>255</v>
+        <v>656</v>
       </c>
       <c r="F47" t="n">
-        <v>147</v>
-      </c>
-      <c s="8" r="G47" t="n">
-        <v>0.63</v>
+        <v>394</v>
+      </c>
+      <c s="14" r="G47" t="n">
+        <v>0.62</v>
       </c>
       <c r="H47" t="n">
-        <v>2.93</v>
+        <v>1.14</v>
       </c>
       <c r="I47" t="s">
         <v>41</v>
@@ -2785,28 +2818,28 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B48" t="n">
-        <v>152.61</v>
-      </c>
-      <c s="9" r="C48" t="n">
-        <v>-2.19</v>
-      </c>
-      <c s="9" r="D48" t="n">
-        <v>-1.44</v>
+        <v>222.91</v>
+      </c>
+      <c s="15" r="C48" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c s="15" r="D48" t="n">
+        <v>-0.03</v>
       </c>
       <c r="E48" t="n">
-        <v>599</v>
+        <v>656</v>
       </c>
       <c r="F48" t="n">
-        <v>414</v>
-      </c>
-      <c s="8" r="G48" t="n">
-        <v>0.59</v>
+        <v>394</v>
+      </c>
+      <c s="16" r="G48" t="n">
+        <v>0.62</v>
       </c>
       <c r="H48" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
       <c r="I48" t="s">
         <v>41</v>
@@ -2814,28 +2847,28 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B49" t="n">
-        <v>150.99</v>
-      </c>
-      <c s="10" r="C49" t="n">
-        <v>-3.81</v>
-      </c>
-      <c s="10" r="D49" t="n">
-        <v>-2.52</v>
+        <v>222.97</v>
+      </c>
+      <c s="17" r="C49" t="n">
+        <v>-0.01</v>
+      </c>
+      <c s="18" r="D49" t="n">
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>823</v>
+        <v>656</v>
       </c>
       <c r="F49" t="n">
-        <v>612</v>
-      </c>
-      <c s="11" r="G49" t="n">
-        <v>0.57</v>
+        <v>394</v>
+      </c>
+      <c s="18" r="G49" t="n">
+        <v>0.62</v>
       </c>
       <c r="H49" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
       <c r="I49" t="s">
         <v>41</v>
@@ -2843,28 +2876,28 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50" t="n">
-        <v>150.54</v>
-      </c>
-      <c s="10" r="C50" t="n">
-        <v>-4.25</v>
-      </c>
-      <c s="10" r="D50" t="n">
-        <v>-2.82</v>
+        <v>223.05</v>
+      </c>
+      <c s="22" r="C50" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c s="22" r="D50" t="n">
+        <v>0.03</v>
       </c>
       <c r="E50" t="n">
-        <v>823</v>
+        <v>807</v>
       </c>
       <c r="F50" t="n">
-        <v>612</v>
-      </c>
-      <c s="11" r="G50" t="n">
-        <v>0.57</v>
+        <v>463</v>
+      </c>
+      <c s="22" r="G50" t="n">
+        <v>0.64</v>
       </c>
       <c r="H50" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
       <c r="I50" t="s">
         <v>41</v>
@@ -2872,28 +2905,28 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B51" t="n">
-        <v>150.46</v>
-      </c>
-      <c s="10" r="C51" t="n">
-        <v>-4.34</v>
-      </c>
-      <c s="10" r="D51" t="n">
-        <v>-2.88</v>
+        <v>223.19</v>
+      </c>
+      <c s="24" r="C51" t="n">
+        <v>0.21</v>
+      </c>
+      <c s="24" r="D51" t="n">
+        <v>0.09</v>
       </c>
       <c r="E51" t="n">
-        <v>823</v>
+        <v>807</v>
       </c>
       <c r="F51" t="n">
-        <v>612</v>
-      </c>
-      <c s="11" r="G51" t="n">
-        <v>0.57</v>
+        <v>463</v>
+      </c>
+      <c s="24" r="G51" t="n">
+        <v>0.64</v>
       </c>
       <c r="H51" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
       <c r="I51" t="s">
         <v>41</v>
@@ -2901,28 +2934,28 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B52" t="n">
-        <v>150.12</v>
-      </c>
-      <c s="10" r="C52" t="n">
-        <v>-4.68</v>
-      </c>
-      <c s="10" r="D52" t="n">
-        <v>-3.12</v>
+        <v>223.18</v>
+      </c>
+      <c s="24" r="C52" t="n">
+        <v>0.2</v>
+      </c>
+      <c s="24" r="D52" t="n">
+        <v>0.09</v>
       </c>
       <c r="E52" t="n">
-        <v>823</v>
+        <v>807</v>
       </c>
       <c r="F52" t="n">
-        <v>612</v>
-      </c>
-      <c s="11" r="G52" t="n">
-        <v>0.57</v>
+        <v>463</v>
+      </c>
+      <c s="24" r="G52" t="n">
+        <v>0.64</v>
       </c>
       <c r="H52" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
       <c r="I52" t="s">
         <v>41</v>
@@ -2930,28 +2963,28 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B53" t="n">
-        <v>150.31</v>
-      </c>
-      <c s="17" r="C53" t="n">
-        <v>-4.49</v>
-      </c>
-      <c s="17" r="D53" t="n">
-        <v>-2.99</v>
+        <v>223.68</v>
+      </c>
+      <c s="24" r="C53" t="n">
+        <v>0.7</v>
+      </c>
+      <c s="24" r="D53" t="n">
+        <v>0.31</v>
       </c>
       <c r="E53" t="n">
-        <v>916</v>
+        <v>970</v>
       </c>
       <c r="F53" t="n">
-        <v>660</v>
-      </c>
-      <c s="18" r="G53" t="n">
-        <v>0.58</v>
+        <v>546</v>
+      </c>
+      <c s="24" r="G53" t="n">
+        <v>0.64</v>
       </c>
       <c r="H53" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
       <c r="I53" t="s">
         <v>41</v>
@@ -2959,28 +2992,28 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B54" t="n">
-        <v>150.17</v>
-      </c>
-      <c s="19" r="C54" t="n">
-        <v>-4.63</v>
-      </c>
-      <c s="19" r="D54" t="n">
-        <v>-3.08</v>
+        <v>223.78</v>
+      </c>
+      <c s="24" r="C54" t="n">
+        <v>0.8</v>
+      </c>
+      <c s="24" r="D54" t="n">
+        <v>0.36</v>
       </c>
       <c r="E54" t="n">
-        <v>916</v>
+        <v>970</v>
       </c>
       <c r="F54" t="n">
-        <v>660</v>
-      </c>
-      <c s="20" r="G54" t="n">
-        <v>0.58</v>
+        <v>546</v>
+      </c>
+      <c s="24" r="G54" t="n">
+        <v>0.64</v>
       </c>
       <c r="H54" t="n">
-        <v>1.13</v>
+        <v>1.14</v>
       </c>
       <c r="I54" t="s">
         <v>41</v>
@@ -2988,480 +3021,1350 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" t="n">
+        <v>224.41</v>
+      </c>
+      <c s="26" r="C55" t="n">
+        <v>1.43</v>
+      </c>
+      <c s="26" r="D55" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="E55" t="n">
+        <v>970</v>
+      </c>
+      <c r="F55" t="n">
+        <v>546</v>
+      </c>
+      <c s="26" r="G55" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="H55" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I55" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" t="n">
+        <v>25.2</v>
+      </c>
+      <c s="8" r="C56" t="n">
+        <v>0.15</v>
+      </c>
+      <c s="8" r="D56" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2477</v>
+      </c>
+      <c r="F56" t="n">
+        <v>2465</v>
+      </c>
+      <c s="8" r="G56" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H56" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" t="n">
+        <v>25.2</v>
+      </c>
+      <c s="8" r="C57" t="n">
+        <v>0.15</v>
+      </c>
+      <c s="8" r="D57" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2477</v>
+      </c>
+      <c r="F57" t="n">
+        <v>2465</v>
+      </c>
+      <c s="8" r="G57" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H57" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I57" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" t="n">
+        <v>24.98</v>
+      </c>
+      <c s="10" r="C58" t="n">
+        <v>-0.22</v>
+      </c>
+      <c s="10" r="D58" t="n">
+        <v>-0.88</v>
+      </c>
+      <c r="E58" t="n">
+        <v>449</v>
+      </c>
+      <c r="F58" t="n">
+        <v>306</v>
+      </c>
+      <c s="11" r="G58" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H58" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I58" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" t="n">
+        <v>24.99</v>
+      </c>
+      <c s="10" r="C59" t="n">
+        <v>-0.21</v>
+      </c>
+      <c s="10" r="D59" t="n">
+        <v>-0.84</v>
+      </c>
+      <c r="E59" t="n">
+        <v>449</v>
+      </c>
+      <c r="F59" t="n">
+        <v>306</v>
+      </c>
+      <c s="11" r="G59" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H59" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="n">
+        <v>25.04</v>
+      </c>
+      <c s="10" r="C60" t="n">
+        <v>-0.16</v>
+      </c>
+      <c s="10" r="D60" t="n">
+        <v>-0.64</v>
+      </c>
+      <c r="E60" t="n">
+        <v>449</v>
+      </c>
+      <c r="F60" t="n">
+        <v>306</v>
+      </c>
+      <c s="11" r="G60" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H60" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I60" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="n">
+        <v>25.1</v>
+      </c>
+      <c s="10" r="C61" t="n">
+        <v>-0.1</v>
+      </c>
+      <c s="10" r="D61" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="E61" t="n">
+        <v>449</v>
+      </c>
+      <c r="F61" t="n">
+        <v>306</v>
+      </c>
+      <c s="11" r="G61" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H61" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I61" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="n">
+        <v>25.25</v>
+      </c>
+      <c s="14" r="C62" t="n">
+        <v>0.05</v>
+      </c>
+      <c s="14" r="D62" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E62" t="n">
+        <v>537</v>
+      </c>
+      <c r="F62" t="n">
+        <v>375</v>
+      </c>
+      <c s="14" r="G62" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H62" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I62" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="n">
+        <v>25.33</v>
+      </c>
+      <c s="16" r="C63" t="n">
+        <v>0.13</v>
+      </c>
+      <c s="16" r="D63" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E63" t="n">
+        <v>537</v>
+      </c>
+      <c r="F63" t="n">
+        <v>375</v>
+      </c>
+      <c s="16" r="G63" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H63" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I63" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="n">
+        <v>25.25</v>
+      </c>
+      <c s="18" r="C64" t="n">
+        <v>0.05</v>
+      </c>
+      <c s="18" r="D64" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E64" t="n">
+        <v>537</v>
+      </c>
+      <c r="F64" t="n">
+        <v>375</v>
+      </c>
+      <c s="18" r="G64" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H64" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I64" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="n">
+        <v>25.57</v>
+      </c>
+      <c s="22" r="C65" t="n">
+        <v>0.38</v>
+      </c>
+      <c s="22" r="D65" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="E65" t="n">
+        <v>747</v>
+      </c>
+      <c r="F65" t="n">
+        <v>588</v>
+      </c>
+      <c s="22" r="G65" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H65" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I65" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" t="n">
+        <v>25.57</v>
+      </c>
+      <c s="24" r="C66" t="n">
+        <v>0.38</v>
+      </c>
+      <c s="24" r="D66" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="E66" t="n">
+        <v>747</v>
+      </c>
+      <c r="F66" t="n">
+        <v>588</v>
+      </c>
+      <c s="24" r="G66" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H66" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I66" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" t="n">
+        <v>25.59</v>
+      </c>
+      <c s="24" r="C67" t="n">
+        <v>0.39</v>
+      </c>
+      <c s="24" r="D67" t="n">
+        <v>1.52</v>
+      </c>
+      <c r="E67" t="n">
+        <v>747</v>
+      </c>
+      <c r="F67" t="n">
+        <v>588</v>
+      </c>
+      <c s="24" r="G67" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H67" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I67" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" t="n">
+        <v>25.19</v>
+      </c>
+      <c s="23" r="C68" t="n">
+        <v>-0.01</v>
+      </c>
+      <c s="23" r="D68" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="E68" t="n">
+        <v>913</v>
+      </c>
+      <c r="F68" t="n">
+        <v>727</v>
+      </c>
+      <c s="24" r="G68" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H68" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I68" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B69" t="n">
+        <v>25.16</v>
+      </c>
+      <c s="23" r="C69" t="n">
+        <v>-0.04</v>
+      </c>
+      <c s="23" r="D69" t="n">
+        <v>-0.16</v>
+      </c>
+      <c r="E69" t="n">
+        <v>913</v>
+      </c>
+      <c r="F69" t="n">
+        <v>727</v>
+      </c>
+      <c s="24" r="G69" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H69" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I69" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" t="n">
+        <v>25.33</v>
+      </c>
+      <c s="26" r="C70" t="n">
+        <v>0.13</v>
+      </c>
+      <c s="26" r="D70" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E70" t="n">
+        <v>913</v>
+      </c>
+      <c r="F70" t="n">
+        <v>727</v>
+      </c>
+      <c s="26" r="G70" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H70" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="I70" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" t="n">
+        <v>44.69</v>
+      </c>
+      <c s="9" r="C71" t="n">
+        <v>-1.71</v>
+      </c>
+      <c s="9" r="D71" t="n">
+        <v>-3.83</v>
+      </c>
+      <c r="E71" t="n">
+        <v>255</v>
+      </c>
+      <c r="F71" t="n">
+        <v>147</v>
+      </c>
+      <c s="8" r="G71" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="H71" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="I71" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
         <v>13</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B72" t="n">
+        <v>152.61</v>
+      </c>
+      <c s="9" r="C72" t="n">
+        <v>-2.19</v>
+      </c>
+      <c s="9" r="D72" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="E72" t="n">
+        <v>599</v>
+      </c>
+      <c r="F72" t="n">
+        <v>414</v>
+      </c>
+      <c s="8" r="G72" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H72" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I72" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>13</v>
+      </c>
+      <c r="B73" t="n">
+        <v>150.99</v>
+      </c>
+      <c s="10" r="C73" t="n">
+        <v>-3.81</v>
+      </c>
+      <c s="10" r="D73" t="n">
+        <v>-2.52</v>
+      </c>
+      <c r="E73" t="n">
+        <v>823</v>
+      </c>
+      <c r="F73" t="n">
+        <v>612</v>
+      </c>
+      <c s="11" r="G73" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H73" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I73" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" t="n">
+        <v>150.54</v>
+      </c>
+      <c s="10" r="C74" t="n">
+        <v>-4.25</v>
+      </c>
+      <c s="10" r="D74" t="n">
+        <v>-2.82</v>
+      </c>
+      <c r="E74" t="n">
+        <v>823</v>
+      </c>
+      <c r="F74" t="n">
+        <v>612</v>
+      </c>
+      <c s="11" r="G74" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H74" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I74" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" t="n">
+        <v>150.46</v>
+      </c>
+      <c s="10" r="C75" t="n">
+        <v>-4.34</v>
+      </c>
+      <c s="10" r="D75" t="n">
+        <v>-2.88</v>
+      </c>
+      <c r="E75" t="n">
+        <v>823</v>
+      </c>
+      <c r="F75" t="n">
+        <v>612</v>
+      </c>
+      <c s="11" r="G75" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I75" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>13</v>
+      </c>
+      <c r="B76" t="n">
+        <v>150.12</v>
+      </c>
+      <c s="10" r="C76" t="n">
+        <v>-4.68</v>
+      </c>
+      <c s="10" r="D76" t="n">
+        <v>-3.12</v>
+      </c>
+      <c r="E76" t="n">
+        <v>823</v>
+      </c>
+      <c r="F76" t="n">
+        <v>612</v>
+      </c>
+      <c s="11" r="G76" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I76" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" t="n">
+        <v>150.31</v>
+      </c>
+      <c s="13" r="C77" t="n">
+        <v>-4.49</v>
+      </c>
+      <c s="13" r="D77" t="n">
+        <v>-2.99</v>
+      </c>
+      <c r="E77" t="n">
+        <v>916</v>
+      </c>
+      <c r="F77" t="n">
+        <v>660</v>
+      </c>
+      <c s="14" r="G77" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H77" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I77" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" t="n">
+        <v>150.17</v>
+      </c>
+      <c s="15" r="C78" t="n">
+        <v>-4.63</v>
+      </c>
+      <c s="15" r="D78" t="n">
+        <v>-3.08</v>
+      </c>
+      <c r="E78" t="n">
+        <v>916</v>
+      </c>
+      <c r="F78" t="n">
+        <v>660</v>
+      </c>
+      <c s="16" r="G78" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H78" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I78" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" t="n">
         <v>150.19</v>
       </c>
-      <c s="21" r="C55" t="n">
+      <c s="17" r="C79" t="n">
         <v>-4.61</v>
       </c>
-      <c s="21" r="D55" t="n">
+      <c s="17" r="D79" t="n">
         <v>-3.07</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E79" t="n">
         <v>916</v>
       </c>
-      <c r="F55" t="n">
+      <c r="F79" t="n">
         <v>660</v>
       </c>
-      <c s="22" r="G55" t="n">
+      <c s="18" r="G79" t="n">
         <v>0.58</v>
       </c>
-      <c r="H55" t="n">
+      <c r="H79" t="n">
         <v>1.13</v>
       </c>
-      <c r="I55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
-      <c s="6" r="C56" t="n"/>
-      <c s="6" r="D56" t="n"/>
-      <c s="5" r="G56" t="n"/>
-    </row>
-    <row r="57" spans="1:9">
-      <c s="6" r="C57" t="n"/>
-      <c s="6" r="D57" t="n"/>
-      <c s="6" r="G57" t="n"/>
-    </row>
-    <row r="58" spans="1:9">
-      <c s="7" r="C58" t="n"/>
-      <c s="7" r="D58" t="n"/>
-      <c s="7" r="G58" t="n"/>
-    </row>
-    <row r="59" spans="1:9">
-      <c s="6" r="C59" t="n"/>
-      <c s="6" r="D59" t="n"/>
-      <c s="5" r="G59" t="n"/>
-    </row>
-    <row r="60" spans="1:9">
-      <c s="6" r="C60" t="n"/>
-      <c s="6" r="D60" t="n"/>
-      <c s="6" r="G60" t="n"/>
-    </row>
-    <row r="61" spans="1:9">
-      <c s="6" r="C61" t="n"/>
-      <c s="6" r="D61" t="n"/>
-      <c s="6" r="G61" t="n"/>
-    </row>
-    <row r="62" spans="1:9">
-      <c s="5" r="C62" t="n"/>
-      <c s="5" r="D62" t="n"/>
-      <c s="6" r="G62" t="n"/>
-    </row>
-    <row r="63" spans="1:9">
-      <c s="5" r="C63" t="n"/>
-      <c s="5" r="D63" t="n"/>
-      <c s="6" r="G63" t="n"/>
-    </row>
-    <row r="64" spans="1:9">
-      <c s="5" r="C64" t="n"/>
-      <c s="5" r="D64" t="n"/>
-      <c s="5" r="G64" t="n"/>
-    </row>
-    <row r="65" spans="1:9">
-      <c s="6" r="C65" t="n"/>
-      <c s="6" r="D65" t="n"/>
-      <c s="6" r="G65" t="n"/>
-    </row>
-    <row r="66" spans="1:9">
-      <c s="6" r="C66" t="n"/>
-      <c s="6" r="D66" t="n"/>
-      <c s="6" r="G66" t="n"/>
-    </row>
-    <row r="67" spans="1:9">
-      <c s="7" r="C67" t="n"/>
-      <c s="7" r="D67" t="n"/>
-      <c s="7" r="G67" t="n"/>
-    </row>
-    <row r="68" spans="1:9">
-      <c s="5" r="C68" t="n"/>
-      <c s="5" r="D68" t="n"/>
-      <c s="5" r="G68" t="n"/>
-    </row>
-    <row r="69" spans="1:9">
-      <c s="6" r="C69" t="n"/>
-      <c s="6" r="D69" t="n"/>
-      <c s="5" r="G69" t="n"/>
-    </row>
-    <row r="70" spans="1:9">
-      <c s="6" r="C70" t="n"/>
-      <c s="6" r="D70" t="n"/>
-      <c s="6" r="G70" t="n"/>
-    </row>
-    <row r="71" spans="1:9">
-      <c s="6" r="C71" t="n"/>
-      <c s="6" r="D71" t="n"/>
-      <c s="6" r="G71" t="n"/>
-    </row>
-    <row r="72" spans="1:9">
-      <c s="5" r="C72" t="n"/>
-      <c s="5" r="D72" t="n"/>
-      <c s="6" r="G72" t="n"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c s="6" r="C73" t="n"/>
-      <c s="6" r="D73" t="n"/>
-      <c s="6" r="G73" t="n"/>
-    </row>
-    <row r="74" spans="1:9">
-      <c s="7" r="C74" t="n"/>
-      <c s="7" r="D74" t="n"/>
-      <c s="7" r="G74" t="n"/>
-    </row>
-    <row r="75" spans="1:9">
-      <c s="5" r="C75" t="n"/>
-      <c s="5" r="D75" t="n"/>
-      <c s="6" r="G75" t="n"/>
-    </row>
-    <row r="76" spans="1:9">
-      <c s="6" r="C76" t="n"/>
-      <c s="6" r="D76" t="n"/>
-      <c s="5" r="G76" t="n"/>
-    </row>
-    <row r="77" spans="1:9">
-      <c s="6" r="C77" t="n"/>
-      <c s="6" r="D77" t="n"/>
-      <c s="6" r="G77" t="n"/>
-    </row>
-    <row r="78" spans="1:9">
-      <c s="6" r="C78" t="n"/>
-      <c s="6" r="D78" t="n"/>
-      <c s="5" r="G78" t="n"/>
-    </row>
-    <row r="79" spans="1:9">
-      <c s="5" r="C79" t="n"/>
-      <c s="5" r="D79" t="n"/>
-      <c s="6" r="G79" t="n"/>
+      <c r="I79" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="80" spans="1:9">
-      <c s="1" r="C80" t="n"/>
-      <c s="1" r="D80" t="n"/>
-      <c s="2" r="G80" t="n"/>
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" t="n">
+        <v>151.79</v>
+      </c>
+      <c s="21" r="C80" t="n">
+        <v>-3.01</v>
+      </c>
+      <c s="21" r="D80" t="n">
+        <v>-1.98</v>
+      </c>
+      <c r="E80" t="n">
+        <v>1038</v>
+      </c>
+      <c r="F80" t="n">
+        <v>736</v>
+      </c>
+      <c s="22" r="G80" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H80" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I80" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="81" spans="1:9">
-      <c s="2" r="C81" t="n"/>
-      <c s="2" r="D81" t="n"/>
-      <c s="2" r="G81" t="n"/>
+      <c r="A81" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" t="n">
+        <v>152.28</v>
+      </c>
+      <c s="23" r="C81" t="n">
+        <v>-2.52</v>
+      </c>
+      <c s="23" r="D81" t="n">
+        <v>-1.65</v>
+      </c>
+      <c r="E81" t="n">
+        <v>1038</v>
+      </c>
+      <c r="F81" t="n">
+        <v>736</v>
+      </c>
+      <c s="24" r="G81" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H81" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I81" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="82" spans="1:9">
-      <c s="1" r="C82" t="n"/>
-      <c s="1" r="D82" t="n"/>
-      <c s="2" r="G82" t="n"/>
+      <c r="A82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" t="n">
+        <v>152.03</v>
+      </c>
+      <c s="23" r="C82" t="n">
+        <v>-2.77</v>
+      </c>
+      <c s="23" r="D82" t="n">
+        <v>-1.82</v>
+      </c>
+      <c r="E82" t="n">
+        <v>1038</v>
+      </c>
+      <c r="F82" t="n">
+        <v>736</v>
+      </c>
+      <c s="24" r="G82" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H82" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I82" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="83" spans="1:9">
-      <c s="2" r="C83" t="n"/>
-      <c s="2" r="D83" t="n"/>
-      <c s="2" r="G83" t="n"/>
+      <c r="A83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" t="n">
+        <v>152.02</v>
+      </c>
+      <c s="23" r="C83" t="n">
+        <v>-2.78</v>
+      </c>
+      <c s="23" r="D83" t="n">
+        <v>-1.83</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1112</v>
+      </c>
+      <c r="F83" t="n">
+        <v>787</v>
+      </c>
+      <c s="24" r="G83" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H83" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I83" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="84" spans="1:9">
-      <c s="2" r="C84" t="n"/>
-      <c s="2" r="D84" t="n"/>
-      <c s="2" r="G84" t="n"/>
+      <c r="A84" t="s">
+        <v>13</v>
+      </c>
+      <c r="B84" t="n">
+        <v>151.68</v>
+      </c>
+      <c s="23" r="C84" t="n">
+        <v>-3.12</v>
+      </c>
+      <c s="23" r="D84" t="n">
+        <v>-2.06</v>
+      </c>
+      <c r="E84" t="n">
+        <v>1112</v>
+      </c>
+      <c r="F84" t="n">
+        <v>787</v>
+      </c>
+      <c s="24" r="G84" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H84" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I84" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="85" spans="1:9">
-      <c s="2" r="C85" t="n"/>
-      <c s="2" r="D85" t="n"/>
-      <c s="2" r="G85" t="n"/>
+      <c r="A85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85" t="n">
+        <v>151.82</v>
+      </c>
+      <c s="25" r="C85" t="n">
+        <v>-2.98</v>
+      </c>
+      <c s="25" r="D85" t="n">
+        <v>-1.96</v>
+      </c>
+      <c r="E85" t="n">
+        <v>1112</v>
+      </c>
+      <c r="F85" t="n">
+        <v>787</v>
+      </c>
+      <c s="26" r="G85" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H85" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="I85" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="86" spans="1:9">
-      <c s="1" r="C86" t="n"/>
-      <c s="1" r="D86" t="n"/>
-      <c s="2" r="G86" t="n"/>
+      <c s="6" r="C86" t="n"/>
+      <c s="6" r="D86" t="n"/>
+      <c s="5" r="G86" t="n"/>
     </row>
     <row r="87" spans="1:9">
-      <c s="3" r="C87" t="n"/>
-      <c s="3" r="D87" t="n"/>
-      <c s="4" r="G87" t="n"/>
+      <c s="6" r="C87" t="n"/>
+      <c s="6" r="D87" t="n"/>
+      <c s="6" r="G87" t="n"/>
     </row>
     <row r="88" spans="1:9">
-      <c s="4" r="C88" t="n"/>
-      <c s="4" r="D88" t="n"/>
-      <c s="4" r="G88" t="n"/>
+      <c s="7" r="C88" t="n"/>
+      <c s="7" r="D88" t="n"/>
+      <c s="7" r="G88" t="n"/>
     </row>
     <row r="89" spans="1:9">
-      <c s="3" r="C89" t="n"/>
-      <c s="3" r="D89" t="n"/>
-      <c s="3" r="G89" t="n"/>
+      <c s="6" r="C89" t="n"/>
+      <c s="6" r="D89" t="n"/>
+      <c s="5" r="G89" t="n"/>
     </row>
     <row r="90" spans="1:9">
-      <c s="3" r="C90" t="n"/>
-      <c s="3" r="D90" t="n"/>
-      <c s="3" r="G90" t="n"/>
+      <c s="6" r="C90" t="n"/>
+      <c s="6" r="D90" t="n"/>
+      <c s="6" r="G90" t="n"/>
     </row>
     <row r="91" spans="1:9">
-      <c s="4" r="C91" t="n"/>
-      <c s="4" r="D91" t="n"/>
-      <c s="4" r="G91" t="n"/>
+      <c s="6" r="C91" t="n"/>
+      <c s="6" r="D91" t="n"/>
+      <c s="6" r="G91" t="n"/>
     </row>
     <row r="92" spans="1:9">
-      <c s="4" r="C92" t="n"/>
-      <c s="4" r="D92" t="n"/>
-      <c s="4" r="G92" t="n"/>
+      <c s="5" r="C92" t="n"/>
+      <c s="5" r="D92" t="n"/>
+      <c s="6" r="G92" t="n"/>
     </row>
     <row r="93" spans="1:9">
-      <c s="4" r="C93" t="n"/>
-      <c s="4" r="D93" t="n"/>
-      <c s="4" r="G93" t="n"/>
+      <c s="5" r="C93" t="n"/>
+      <c s="5" r="D93" t="n"/>
+      <c s="6" r="G93" t="n"/>
     </row>
     <row r="94" spans="1:9">
-      <c s="3" r="C94" t="n"/>
-      <c s="3" r="D94" t="n"/>
-      <c s="3" r="G94" t="n"/>
+      <c s="5" r="C94" t="n"/>
+      <c s="5" r="D94" t="n"/>
+      <c s="5" r="G94" t="n"/>
     </row>
     <row r="95" spans="1:9">
-      <c s="4" r="C95" t="n"/>
-      <c s="4" r="D95" t="n"/>
-      <c s="3" r="G95" t="n"/>
+      <c s="6" r="C95" t="n"/>
+      <c s="6" r="D95" t="n"/>
+      <c s="6" r="G95" t="n"/>
     </row>
     <row r="96" spans="1:9">
-      <c s="4" r="C96" t="n"/>
-      <c s="4" r="D96" t="n"/>
-      <c s="3" r="G96" t="n"/>
+      <c s="6" r="C96" t="n"/>
+      <c s="6" r="D96" t="n"/>
+      <c s="6" r="G96" t="n"/>
     </row>
     <row r="97" spans="1:9">
-      <c s="4" r="C97" t="n"/>
-      <c s="4" r="D97" t="n"/>
-      <c s="4" r="G97" t="n"/>
+      <c s="7" r="C97" t="n"/>
+      <c s="7" r="D97" t="n"/>
+      <c s="7" r="G97" t="n"/>
     </row>
     <row r="98" spans="1:9">
-      <c s="4" r="C98" t="n"/>
-      <c s="4" r="D98" t="n"/>
-      <c s="3" r="G98" t="n"/>
+      <c s="5" r="C98" t="n"/>
+      <c s="5" r="D98" t="n"/>
+      <c s="5" r="G98" t="n"/>
     </row>
     <row r="99" spans="1:9">
-      <c s="4" r="C99" t="n"/>
-      <c s="4" r="D99" t="n"/>
-      <c s="4" r="G99" t="n"/>
+      <c s="6" r="C99" t="n"/>
+      <c s="6" r="D99" t="n"/>
+      <c s="5" r="G99" t="n"/>
     </row>
     <row r="100" spans="1:9">
-      <c s="4" r="C100" t="n"/>
-      <c s="4" r="D100" t="n"/>
-      <c s="4" r="G100" t="n"/>
+      <c s="6" r="C100" t="n"/>
+      <c s="6" r="D100" t="n"/>
+      <c s="6" r="G100" t="n"/>
     </row>
     <row r="101" spans="1:9">
-      <c s="3" r="C101" t="n"/>
-      <c s="3" r="D101" t="n"/>
-      <c s="4" r="G101" t="n"/>
+      <c s="6" r="C101" t="n"/>
+      <c s="6" r="D101" t="n"/>
+      <c s="6" r="G101" t="n"/>
     </row>
     <row r="102" spans="1:9">
-      <c s="3" r="C102" t="n"/>
-      <c s="3" r="D102" t="n"/>
-      <c s="4" r="G102" t="n"/>
+      <c s="5" r="C102" t="n"/>
+      <c s="5" r="D102" t="n"/>
+      <c s="6" r="G102" t="n"/>
     </row>
     <row r="103" spans="1:9">
-      <c s="3" r="C103" t="n"/>
-      <c s="3" r="D103" t="n"/>
-      <c s="3" r="G103" t="n"/>
+      <c s="6" r="C103" t="n"/>
+      <c s="6" r="D103" t="n"/>
+      <c s="6" r="G103" t="n"/>
     </row>
     <row r="104" spans="1:9">
-      <c s="4" r="C104" t="n"/>
-      <c s="4" r="D104" t="n"/>
-      <c s="4" r="G104" t="n"/>
+      <c s="7" r="C104" t="n"/>
+      <c s="7" r="D104" t="n"/>
+      <c s="7" r="G104" t="n"/>
     </row>
     <row r="105" spans="1:9">
-      <c s="4" r="C105" t="n"/>
-      <c s="4" r="D105" t="n"/>
-      <c s="4" r="G105" t="n"/>
+      <c s="5" r="C105" t="n"/>
+      <c s="5" r="D105" t="n"/>
+      <c s="6" r="G105" t="n"/>
     </row>
     <row r="106" spans="1:9">
-      <c s="3" r="C106" t="n"/>
-      <c s="3" r="D106" t="n"/>
-      <c s="3" r="G106" t="n"/>
+      <c s="6" r="C106" t="n"/>
+      <c s="6" r="D106" t="n"/>
+      <c s="5" r="G106" t="n"/>
     </row>
     <row r="107" spans="1:9">
-      <c s="4" r="C107" t="n"/>
-      <c s="4" r="D107" t="n"/>
-      <c s="3" r="G107" t="n"/>
+      <c s="6" r="C107" t="n"/>
+      <c s="6" r="D107" t="n"/>
+      <c s="6" r="G107" t="n"/>
     </row>
     <row r="108" spans="1:9">
-      <c s="4" r="C108" t="n"/>
-      <c s="4" r="D108" t="n"/>
-      <c s="4" r="G108" t="n"/>
+      <c s="6" r="C108" t="n"/>
+      <c s="6" r="D108" t="n"/>
+      <c s="5" r="G108" t="n"/>
     </row>
     <row r="109" spans="1:9">
-      <c s="4" r="C109" t="n"/>
-      <c s="4" r="D109" t="n"/>
-      <c s="4" r="G109" t="n"/>
+      <c s="5" r="C109" t="n"/>
+      <c s="5" r="D109" t="n"/>
+      <c s="6" r="G109" t="n"/>
     </row>
     <row r="110" spans="1:9">
-      <c s="3" r="C110" t="n"/>
-      <c s="3" r="D110" t="n"/>
-      <c s="4" r="G110" t="n"/>
+      <c s="1" r="C110" t="n"/>
+      <c s="1" r="D110" t="n"/>
+      <c s="2" r="G110" t="n"/>
     </row>
     <row r="111" spans="1:9">
-      <c s="4" r="C111" t="n"/>
-      <c s="4" r="D111" t="n"/>
-      <c s="4" r="G111" t="n"/>
+      <c s="2" r="C111" t="n"/>
+      <c s="2" r="D111" t="n"/>
+      <c s="2" r="G111" t="n"/>
     </row>
     <row r="112" spans="1:9">
-      <c s="3" r="C112" t="n"/>
-      <c s="3" r="D112" t="n"/>
-      <c s="4" r="G112" t="n"/>
+      <c s="1" r="C112" t="n"/>
+      <c s="1" r="D112" t="n"/>
+      <c s="2" r="G112" t="n"/>
     </row>
     <row r="113" spans="1:9">
-      <c s="4" r="C113" t="n"/>
-      <c s="4" r="D113" t="n"/>
-      <c s="3" r="G113" t="n"/>
+      <c s="2" r="C113" t="n"/>
+      <c s="2" r="D113" t="n"/>
+      <c s="2" r="G113" t="n"/>
     </row>
     <row r="114" spans="1:9">
-      <c s="4" r="C114" t="n"/>
-      <c s="4" r="D114" t="n"/>
-      <c s="4" r="G114" t="n"/>
+      <c s="2" r="C114" t="n"/>
+      <c s="2" r="D114" t="n"/>
+      <c s="2" r="G114" t="n"/>
     </row>
     <row r="115" spans="1:9">
-      <c s="4" r="C115" t="n"/>
-      <c s="4" r="D115" t="n"/>
-      <c s="3" r="G115" t="n"/>
+      <c s="2" r="C115" t="n"/>
+      <c s="2" r="D115" t="n"/>
+      <c s="2" r="G115" t="n"/>
     </row>
     <row r="116" spans="1:9">
-      <c s="3" r="C116" t="n"/>
-      <c s="3" r="D116" t="n"/>
-      <c s="4" r="G116" t="n"/>
+      <c s="1" r="C116" t="n"/>
+      <c s="1" r="D116" t="n"/>
+      <c s="2" r="G116" t="n"/>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" t="s">
+      <c s="3" r="C117" t="n"/>
+      <c s="3" r="D117" t="n"/>
+      <c s="4" r="G117" t="n"/>
+    </row>
+    <row r="118" spans="1:9">
+      <c s="4" r="C118" t="n"/>
+      <c s="4" r="D118" t="n"/>
+      <c s="4" r="G118" t="n"/>
+    </row>
+    <row r="119" spans="1:9">
+      <c s="3" r="C119" t="n"/>
+      <c s="3" r="D119" t="n"/>
+      <c s="3" r="G119" t="n"/>
+    </row>
+    <row r="120" spans="1:9">
+      <c s="3" r="C120" t="n"/>
+      <c s="3" r="D120" t="n"/>
+      <c s="3" r="G120" t="n"/>
+    </row>
+    <row r="121" spans="1:9">
+      <c s="4" r="C121" t="n"/>
+      <c s="4" r="D121" t="n"/>
+      <c s="4" r="G121" t="n"/>
+    </row>
+    <row r="122" spans="1:9">
+      <c s="4" r="C122" t="n"/>
+      <c s="4" r="D122" t="n"/>
+      <c s="4" r="G122" t="n"/>
+    </row>
+    <row r="123" spans="1:9">
+      <c s="4" r="C123" t="n"/>
+      <c s="4" r="D123" t="n"/>
+      <c s="4" r="G123" t="n"/>
+    </row>
+    <row r="124" spans="1:9">
+      <c s="3" r="C124" t="n"/>
+      <c s="3" r="D124" t="n"/>
+      <c s="3" r="G124" t="n"/>
+    </row>
+    <row r="125" spans="1:9">
+      <c s="4" r="C125" t="n"/>
+      <c s="4" r="D125" t="n"/>
+      <c s="3" r="G125" t="n"/>
+    </row>
+    <row r="126" spans="1:9">
+      <c s="4" r="C126" t="n"/>
+      <c s="4" r="D126" t="n"/>
+      <c s="3" r="G126" t="n"/>
+    </row>
+    <row r="127" spans="1:9">
+      <c s="4" r="C127" t="n"/>
+      <c s="4" r="D127" t="n"/>
+      <c s="4" r="G127" t="n"/>
+    </row>
+    <row r="128" spans="1:9">
+      <c s="4" r="C128" t="n"/>
+      <c s="4" r="D128" t="n"/>
+      <c s="3" r="G128" t="n"/>
+    </row>
+    <row r="129" spans="1:9">
+      <c s="4" r="C129" t="n"/>
+      <c s="4" r="D129" t="n"/>
+      <c s="4" r="G129" t="n"/>
+    </row>
+    <row r="130" spans="1:9">
+      <c s="4" r="C130" t="n"/>
+      <c s="4" r="D130" t="n"/>
+      <c s="4" r="G130" t="n"/>
+    </row>
+    <row r="131" spans="1:9">
+      <c s="3" r="C131" t="n"/>
+      <c s="3" r="D131" t="n"/>
+      <c s="4" r="G131" t="n"/>
+    </row>
+    <row r="132" spans="1:9">
+      <c s="3" r="C132" t="n"/>
+      <c s="3" r="D132" t="n"/>
+      <c s="4" r="G132" t="n"/>
+    </row>
+    <row r="133" spans="1:9">
+      <c s="3" r="C133" t="n"/>
+      <c s="3" r="D133" t="n"/>
+      <c s="3" r="G133" t="n"/>
+    </row>
+    <row r="134" spans="1:9">
+      <c s="4" r="C134" t="n"/>
+      <c s="4" r="D134" t="n"/>
+      <c s="4" r="G134" t="n"/>
+    </row>
+    <row r="135" spans="1:9">
+      <c s="4" r="C135" t="n"/>
+      <c s="4" r="D135" t="n"/>
+      <c s="4" r="G135" t="n"/>
+    </row>
+    <row r="136" spans="1:9">
+      <c s="3" r="C136" t="n"/>
+      <c s="3" r="D136" t="n"/>
+      <c s="3" r="G136" t="n"/>
+    </row>
+    <row r="137" spans="1:9">
+      <c s="4" r="C137" t="n"/>
+      <c s="4" r="D137" t="n"/>
+      <c s="3" r="G137" t="n"/>
+    </row>
+    <row r="138" spans="1:9">
+      <c s="4" r="C138" t="n"/>
+      <c s="4" r="D138" t="n"/>
+      <c s="4" r="G138" t="n"/>
+    </row>
+    <row r="139" spans="1:9">
+      <c s="4" r="C139" t="n"/>
+      <c s="4" r="D139" t="n"/>
+      <c s="4" r="G139" t="n"/>
+    </row>
+    <row r="140" spans="1:9">
+      <c s="3" r="C140" t="n"/>
+      <c s="3" r="D140" t="n"/>
+      <c s="4" r="G140" t="n"/>
+    </row>
+    <row r="141" spans="1:9">
+      <c s="4" r="C141" t="n"/>
+      <c s="4" r="D141" t="n"/>
+      <c s="4" r="G141" t="n"/>
+    </row>
+    <row r="142" spans="1:9">
+      <c s="3" r="C142" t="n"/>
+      <c s="3" r="D142" t="n"/>
+      <c s="4" r="G142" t="n"/>
+    </row>
+    <row r="143" spans="1:9">
+      <c s="4" r="C143" t="n"/>
+      <c s="4" r="D143" t="n"/>
+      <c s="3" r="G143" t="n"/>
+    </row>
+    <row r="144" spans="1:9">
+      <c s="4" r="C144" t="n"/>
+      <c s="4" r="D144" t="n"/>
+      <c s="4" r="G144" t="n"/>
+    </row>
+    <row r="145" spans="1:9">
+      <c s="4" r="C145" t="n"/>
+      <c s="4" r="D145" t="n"/>
+      <c s="3" r="G145" t="n"/>
+    </row>
+    <row r="146" spans="1:9">
+      <c s="3" r="C146" t="n"/>
+      <c s="3" r="D146" t="n"/>
+      <c s="4" r="G146" t="n"/>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" t="s">
         <v>9</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B147" t="n">
         <v>12.74</v>
       </c>
-      <c s="8" r="C117" t="n">
+      <c s="8" r="C147" t="n">
         <v>1.66</v>
       </c>
-      <c s="8" r="D117" t="n">
+      <c s="8" r="D147" t="n">
         <v>13.03</v>
       </c>
-      <c r="E117" t="n">
+      <c r="E147" t="n">
         <v>2240</v>
       </c>
-      <c r="F117" t="n">
+      <c r="F147" t="n">
         <v>1400</v>
       </c>
-      <c s="8" r="G117" t="n">
+      <c s="8" r="G147" t="n">
         <v>0.62</v>
       </c>
-      <c r="H117" t="n">
+      <c r="H147" t="n">
         <v>3.95</v>
       </c>
-      <c r="I117" t="s">
+      <c r="I147" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
-      <c r="A118" t="s">
+    <row r="148" spans="1:9">
+      <c r="A148" t="s">
+        <v>10</v>
+      </c>
+      <c r="B148" t="n">
+        <v>1998.1</v>
+      </c>
+      <c s="8" r="C148" t="n">
+        <v>65.28</v>
+      </c>
+      <c s="8" r="D148" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="E148" t="n">
+        <v>2791</v>
+      </c>
+      <c r="F148" t="n">
+        <v>2724</v>
+      </c>
+      <c s="8" r="G148" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="H148" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="I148" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
+      <c r="A149" t="s">
+        <v>17</v>
+      </c>
+      <c r="B149" t="n">
+        <v>62.13</v>
+      </c>
+      <c s="8" r="C149" t="n">
+        <v>10.63</v>
+      </c>
+      <c s="8" r="D149" t="n">
+        <v>17.11</v>
+      </c>
+      <c r="E149" t="n">
+        <v>2390</v>
+      </c>
+      <c r="F149" t="n">
+        <v>1583</v>
+      </c>
+      <c s="8" r="G149" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H149" t="s">
+        <v>18</v>
+      </c>
+      <c r="I149" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
+      <c r="A150" t="s">
         <v>11</v>
       </c>
-      <c r="B118" t="n">
-        <v>1998.1</v>
-      </c>
-      <c s="8" r="C118" t="n">
-        <v>65.28</v>
-      </c>
-      <c s="8" r="D118" t="n">
-        <v>3.27</v>
-      </c>
-      <c r="E118" t="n">
-        <v>2791</v>
-      </c>
-      <c r="F118" t="n">
-        <v>2724</v>
-      </c>
-      <c s="8" r="G118" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="H118" t="n">
-        <v>1.61</v>
-      </c>
-      <c r="I118" t="s">
+      <c r="B150" t="n">
+        <v>222.98</v>
+      </c>
+      <c s="8" r="C150" t="n">
+        <v>3.28</v>
+      </c>
+      <c s="8" r="D150" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="E150" t="n">
+        <v>1715</v>
+      </c>
+      <c r="F150" t="n">
+        <v>1153</v>
+      </c>
+      <c s="8" r="G150" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H150" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="I150" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
-      <c r="A119" t="s">
-        <v>17</v>
-      </c>
-      <c r="B119" t="n">
-        <v>62.13</v>
-      </c>
-      <c s="8" r="C119" t="n">
-        <v>10.63</v>
-      </c>
-      <c s="8" r="D119" t="n">
-        <v>17.11</v>
-      </c>
-      <c r="E119" t="n">
-        <v>2390</v>
-      </c>
-      <c r="F119" t="n">
-        <v>1583</v>
-      </c>
-      <c s="8" r="G119" t="n">
+    <row r="151" spans="1:9">
+      <c r="A151" t="s">
+        <v>12</v>
+      </c>
+      <c r="B151" t="n">
+        <v>25.2</v>
+      </c>
+      <c s="8" r="C151" t="n">
+        <v>0.15</v>
+      </c>
+      <c s="8" r="D151" t="n">
         <v>0.6</v>
       </c>
-      <c r="H119" t="s">
-        <v>18</v>
-      </c>
-      <c r="I119" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
-      <c r="A120" t="s">
-        <v>12</v>
-      </c>
-      <c r="B120" t="n">
-        <v>222.98</v>
-      </c>
-      <c s="8" r="C120" t="n">
-        <v>3.28</v>
-      </c>
-      <c s="8" r="D120" t="n">
-        <v>1.47</v>
-      </c>
-      <c r="E120" t="n">
-        <v>1715</v>
-      </c>
-      <c r="F120" t="n">
-        <v>1153</v>
-      </c>
-      <c s="8" r="G120" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="H120" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="I120" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
-      <c r="A121" t="s">
-        <v>10</v>
-      </c>
-      <c r="B121" t="n">
-        <v>25.2</v>
-      </c>
-      <c s="8" r="C121" t="n">
-        <v>0.15</v>
-      </c>
-      <c s="8" r="D121" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="E121" t="n">
+      <c r="E151" t="n">
         <v>2477</v>
       </c>
-      <c r="F121" t="n">
+      <c r="F151" t="n">
         <v>2465</v>
       </c>
-      <c s="8" r="G121" t="n">
+      <c s="8" r="G151" t="n">
         <v>0.5</v>
       </c>
-      <c r="H121" t="n">
+      <c r="H151" t="n">
         <v>3.6</v>
       </c>
-      <c r="I121" t="s">
+      <c r="I151" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3477,78 +4380,205 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
       <c r="B1" t="s">
         <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c s="12" r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c s="19" r="B2" t="n"/>
+      <c s="20" r="C2" t="n"/>
+      <c s="19" r="D2" t="n"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c s="12" r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c s="19" r="B3" t="n"/>
+      <c s="19" r="C3" t="n"/>
+      <c s="20" r="E3" t="n"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c s="19" r="D4" t="n"/>
+      <c s="19" r="E4" t="n"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c s="12" r="A5" t="s">
         <v>10</v>
       </c>
-      <c s="13" r="B2" t="n"/>
-      <c s="14" r="C2" t="n"/>
-      <c s="15" r="D2" t="n"/>
-      <c s="16" r="E2" t="n"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c s="20" r="E5" t="n"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c s="12" r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c s="19" r="B2" t="n"/>
+      <c s="20" r="C2" t="n"/>
+      <c s="19" r="D2" t="n"/>
+    </row>
+    <row r="3" spans="1:5">
       <c s="12" r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c s="19" r="B3" t="n"/>
+      <c s="19" r="C3" t="n"/>
+      <c s="20" r="E3" t="n"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c s="19" r="D4" t="n"/>
+      <c s="19" r="E4" t="n"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c s="12" r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c s="20" r="E5" t="n"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
         <v>42</v>
       </c>
-      <c s="13" r="B3" t="n"/>
-      <c s="15" r="C3" t="n"/>
-      <c s="14" r="E3" t="n"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c s="12" r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c s="19" r="B2" t="n"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c s="12" r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c s="19" r="B3" t="n"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c s="16" r="C4" t="n"/>
-      <c s="15" r="D4" t="n"/>
-      <c s="15" r="E4" t="n"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c s="12" r="A5" t="s">
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c s="16" r="D5" t="n"/>
-      <c s="14" r="E5" t="n"/>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:3"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>